<commit_message>
Add multiple levels totallabel feature
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
+++ b/tests/Gauges/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <x:si>
     <x:t>Formulas in group row</x:t>
   </x:si>
@@ -48,9 +48,6 @@
   <x:si>
     <x:t>Amount
 paid</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Action Club </x:t>
@@ -1323,9 +1320,7 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <x:c r="B5" s="34" t="s">
-        <x:v>9</x:v>
-      </x:c>
+      <x:c r="B5" s="34" t="s"/>
       <x:c r="C5" s="34" t="s"/>
       <x:c r="D5" s="35" t="s"/>
       <x:c r="E5" s="36" t="s"/>
@@ -1338,7 +1333,7 @@
     </x:row>
     <x:row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <x:c r="B6" s="34" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C6" s="34" t="s"/>
       <x:c r="D6" s="35" t="s"/>
@@ -1354,7 +1349,7 @@
       <x:c r="B7" s="34" t="s"/>
       <x:c r="C7" s="34" t="s"/>
       <x:c r="D7" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E7" s="36" t="s"/>
       <x:c r="F7" s="37" t="s"/>
@@ -1366,13 +1361,13 @@
     </x:row>
     <x:row r="8" spans="1:11" outlineLevel="3">
       <x:c r="B8" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C8" s="41" t="n">
         <x:v>1014</x:v>
       </x:c>
       <x:c r="D8" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E8" s="42">
         <x:v>32289</x:v>
@@ -1394,7 +1389,7 @@
       <x:c r="B9" s="34" t="s"/>
       <x:c r="C9" s="34" t="s"/>
       <x:c r="D9" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E9" s="36" t="s"/>
       <x:c r="F9" s="37" t="s"/>
@@ -1406,13 +1401,13 @@
     </x:row>
     <x:row r="10" spans="1:11" outlineLevel="3">
       <x:c r="B10" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C10" s="41" t="n">
         <x:v>1129</x:v>
       </x:c>
       <x:c r="D10" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E10" s="42">
         <x:v>34261</x:v>
@@ -1432,7 +1427,7 @@
     </x:row>
     <x:row r="11" spans="1:11" outlineLevel="3">
       <x:c r="B11" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C11" s="41" t="n">
         <x:v>1029</x:v>
@@ -1458,7 +1453,7 @@
       <x:c r="B12" s="34" t="s"/>
       <x:c r="C12" s="34" t="s"/>
       <x:c r="D12" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E12" s="36" t="s"/>
       <x:c r="F12" s="37" t="s"/>
@@ -1470,13 +1465,13 @@
     </x:row>
     <x:row r="13" spans="1:11" outlineLevel="3">
       <x:c r="B13" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C13" s="41" t="n">
         <x:v>1038</x:v>
       </x:c>
       <x:c r="D13" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E13" s="42">
         <x:v>32382</x:v>
@@ -1496,7 +1491,7 @@
     </x:row>
     <x:row r="14" spans="1:11" outlineLevel="1">
       <x:c r="B14" s="34" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C14" s="34" t="s"/>
       <x:c r="D14" s="35" t="s"/>
@@ -1512,7 +1507,7 @@
       <x:c r="B15" s="34" t="s"/>
       <x:c r="C15" s="34" t="s"/>
       <x:c r="D15" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E15" s="36" t="s"/>
       <x:c r="F15" s="37" t="s"/>
@@ -1524,13 +1519,13 @@
     </x:row>
     <x:row r="16" spans="1:11" outlineLevel="3">
       <x:c r="B16" s="40" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C16" s="41" t="n">
         <x:v>1039</x:v>
       </x:c>
       <x:c r="D16" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E16" s="42">
         <x:v>32387</x:v>
@@ -1550,7 +1545,7 @@
     </x:row>
     <x:row r="17" spans="1:11" outlineLevel="1">
       <x:c r="B17" s="34" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C17" s="34" t="s"/>
       <x:c r="D17" s="35" t="s"/>
@@ -1566,7 +1561,7 @@
       <x:c r="B18" s="34" t="s"/>
       <x:c r="C18" s="34" t="s"/>
       <x:c r="D18" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E18" s="36" t="s"/>
       <x:c r="F18" s="37" t="s"/>
@@ -1578,13 +1573,13 @@
     </x:row>
     <x:row r="19" spans="1:11" outlineLevel="3">
       <x:c r="B19" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C19" s="41" t="n">
         <x:v>1017</x:v>
       </x:c>
       <x:c r="D19" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E19" s="42">
         <x:v>32307</x:v>
@@ -1604,7 +1599,7 @@
     </x:row>
     <x:row r="20" spans="1:11" outlineLevel="3">
       <x:c r="B20" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C20" s="41" t="n">
         <x:v>1217</x:v>
@@ -1628,7 +1623,7 @@
     </x:row>
     <x:row r="21" spans="1:11" outlineLevel="3">
       <x:c r="B21" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C21" s="41" t="n">
         <x:v>1117</x:v>
@@ -1652,7 +1647,7 @@
     </x:row>
     <x:row r="22" spans="1:11" outlineLevel="3">
       <x:c r="B22" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C22" s="41" t="n">
         <x:v>1317</x:v>
@@ -1678,7 +1673,7 @@
       <x:c r="B23" s="34" t="s"/>
       <x:c r="C23" s="34" t="s"/>
       <x:c r="D23" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E23" s="36" t="s"/>
       <x:c r="F23" s="37" t="s"/>
@@ -1690,13 +1685,13 @@
     </x:row>
     <x:row r="24" spans="1:11" outlineLevel="3">
       <x:c r="B24" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C24" s="41" t="n">
         <x:v>1137</x:v>
       </x:c>
       <x:c r="D24" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E24" s="42">
         <x:v>34300</x:v>
@@ -1716,7 +1711,7 @@
     </x:row>
     <x:row r="25" spans="1:11" outlineLevel="3">
       <x:c r="B25" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C25" s="41" t="n">
         <x:v>1037</x:v>
@@ -1740,7 +1735,7 @@
     </x:row>
     <x:row r="26" spans="1:11" outlineLevel="3">
       <x:c r="B26" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C26" s="41" t="n">
         <x:v>1099</x:v>
@@ -1766,7 +1761,7 @@
       <x:c r="B27" s="34" t="s"/>
       <x:c r="C27" s="34" t="s"/>
       <x:c r="D27" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="36" t="s"/>
       <x:c r="F27" s="37" t="s"/>
@@ -1778,13 +1773,13 @@
     </x:row>
     <x:row r="28" spans="1:11" outlineLevel="3">
       <x:c r="B28" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C28" s="41" t="n">
         <x:v>1294</x:v>
       </x:c>
       <x:c r="D28" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E28" s="42">
         <x:v>34703</x:v>
@@ -1804,7 +1799,7 @@
     </x:row>
     <x:row r="29" spans="1:11" outlineLevel="3">
       <x:c r="B29" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C29" s="41" t="n">
         <x:v>1074</x:v>
@@ -1828,7 +1823,7 @@
     </x:row>
     <x:row r="30" spans="1:11" outlineLevel="1">
       <x:c r="B30" s="34" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C30" s="34" t="s"/>
       <x:c r="D30" s="35" t="s"/>
@@ -1844,7 +1839,7 @@
       <x:c r="B31" s="34" t="s"/>
       <x:c r="C31" s="34" t="s"/>
       <x:c r="D31" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E31" s="36" t="s"/>
       <x:c r="F31" s="37" t="s"/>
@@ -1856,13 +1851,13 @@
     </x:row>
     <x:row r="32" spans="1:11" outlineLevel="3">
       <x:c r="B32" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C32" s="41" t="n">
         <x:v>1204</x:v>
       </x:c>
       <x:c r="D32" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E32" s="42">
         <x:v>34625</x:v>
@@ -1884,7 +1879,7 @@
       <x:c r="B33" s="34" t="s"/>
       <x:c r="C33" s="34" t="s"/>
       <x:c r="D33" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E33" s="36" t="s"/>
       <x:c r="F33" s="37" t="s"/>
@@ -1896,13 +1891,13 @@
     </x:row>
     <x:row r="34" spans="1:11" outlineLevel="3">
       <x:c r="B34" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C34" s="41" t="n">
         <x:v>1355</x:v>
       </x:c>
       <x:c r="D34" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E34" s="42">
         <x:v>34735</x:v>
@@ -1922,7 +1917,7 @@
     </x:row>
     <x:row r="35" spans="1:11" outlineLevel="3">
       <x:c r="B35" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C35" s="41" t="n">
         <x:v>1263</x:v>
@@ -1946,7 +1941,7 @@
     </x:row>
     <x:row r="36" spans="1:11" outlineLevel="1">
       <x:c r="B36" s="34" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C36" s="34" t="s"/>
       <x:c r="D36" s="35" t="s"/>
@@ -1962,7 +1957,7 @@
       <x:c r="B37" s="34" t="s"/>
       <x:c r="C37" s="34" t="s"/>
       <x:c r="D37" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E37" s="36" t="s"/>
       <x:c r="F37" s="37" t="s"/>
@@ -1974,13 +1969,13 @@
     </x:row>
     <x:row r="38" spans="1:11" outlineLevel="3">
       <x:c r="B38" s="40" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C38" s="41" t="n">
         <x:v>1065</x:v>
       </x:c>
       <x:c r="D38" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E38" s="42">
         <x:v>32593</x:v>
@@ -2000,7 +1995,7 @@
     </x:row>
     <x:row r="39" spans="1:11" outlineLevel="1">
       <x:c r="B39" s="34" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C39" s="34" t="s"/>
       <x:c r="D39" s="35" t="s"/>
@@ -2016,7 +2011,7 @@
       <x:c r="B40" s="34" t="s"/>
       <x:c r="C40" s="34" t="s"/>
       <x:c r="D40" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E40" s="36" t="s"/>
       <x:c r="F40" s="37" t="s"/>
@@ -2028,13 +2023,13 @@
     </x:row>
     <x:row r="41" spans="1:11" outlineLevel="3">
       <x:c r="B41" s="40" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C41" s="41" t="n">
         <x:v>1042</x:v>
       </x:c>
       <x:c r="D41" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E41" s="42">
         <x:v>32411</x:v>
@@ -2054,7 +2049,7 @@
     </x:row>
     <x:row r="42" spans="1:11" outlineLevel="3">
       <x:c r="B42" s="40" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C42" s="41" t="n">
         <x:v>1142</x:v>
@@ -2078,7 +2073,7 @@
     </x:row>
     <x:row r="43" spans="1:11" outlineLevel="1">
       <x:c r="B43" s="34" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C43" s="34" t="s"/>
       <x:c r="D43" s="35" t="s"/>
@@ -2094,7 +2089,7 @@
       <x:c r="B44" s="34" t="s"/>
       <x:c r="C44" s="34" t="s"/>
       <x:c r="D44" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E44" s="36" t="s"/>
       <x:c r="F44" s="37" t="s"/>
@@ -2106,13 +2101,13 @@
     </x:row>
     <x:row r="45" spans="1:11" outlineLevel="3">
       <x:c r="B45" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C45" s="41" t="n">
         <x:v>1079</x:v>
       </x:c>
       <x:c r="D45" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E45" s="42">
         <x:v>32632</x:v>
@@ -2132,7 +2127,7 @@
     </x:row>
     <x:row r="46" spans="1:11" outlineLevel="3">
       <x:c r="B46" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C46" s="41" t="n">
         <x:v>1153</x:v>
@@ -2156,7 +2151,7 @@
     </x:row>
     <x:row r="47" spans="1:11" outlineLevel="3">
       <x:c r="B47" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C47" s="41" t="n">
         <x:v>1253</x:v>
@@ -2182,7 +2177,7 @@
       <x:c r="B48" s="34" t="s"/>
       <x:c r="C48" s="34" t="s"/>
       <x:c r="D48" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E48" s="36" t="s"/>
       <x:c r="F48" s="37" t="s"/>
@@ -2194,13 +2189,13 @@
     </x:row>
     <x:row r="49" spans="1:11" outlineLevel="3">
       <x:c r="B49" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C49" s="41" t="n">
         <x:v>1106</x:v>
       </x:c>
       <x:c r="D49" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E49" s="42">
         <x:v>33870</x:v>
@@ -2220,7 +2215,7 @@
     </x:row>
     <x:row r="50" spans="1:11" outlineLevel="3">
       <x:c r="B50" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C50" s="41" t="n">
         <x:v>1006</x:v>
@@ -2244,7 +2239,7 @@
     </x:row>
     <x:row r="51" spans="1:11" outlineLevel="1">
       <x:c r="B51" s="34" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C51" s="34" t="s"/>
       <x:c r="D51" s="35" t="s"/>
@@ -2260,7 +2255,7 @@
       <x:c r="B52" s="34" t="s"/>
       <x:c r="C52" s="34" t="s"/>
       <x:c r="D52" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E52" s="36" t="s"/>
       <x:c r="F52" s="37" t="s"/>
@@ -2272,13 +2267,13 @@
     </x:row>
     <x:row r="53" spans="1:11" outlineLevel="3">
       <x:c r="B53" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C53" s="41" t="n">
         <x:v>1283</x:v>
       </x:c>
       <x:c r="D53" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E53" s="42">
         <x:v>34698</x:v>
@@ -2298,7 +2293,7 @@
     </x:row>
     <x:row r="54" spans="1:11" outlineLevel="3">
       <x:c r="B54" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C54" s="41" t="n">
         <x:v>1083</x:v>
@@ -2324,7 +2319,7 @@
       <x:c r="B55" s="34" t="s"/>
       <x:c r="C55" s="34" t="s"/>
       <x:c r="D55" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E55" s="36" t="s"/>
       <x:c r="F55" s="37" t="s"/>
@@ -2336,13 +2331,13 @@
     </x:row>
     <x:row r="56" spans="1:11" outlineLevel="3">
       <x:c r="B56" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C56" s="41" t="n">
         <x:v>1061</x:v>
       </x:c>
       <x:c r="D56" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E56" s="42">
         <x:v>32571</x:v>
@@ -2362,7 +2357,7 @@
     </x:row>
     <x:row r="57" spans="1:11" outlineLevel="3">
       <x:c r="B57" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C57" s="41" t="n">
         <x:v>1057</x:v>
@@ -2386,7 +2381,7 @@
     </x:row>
     <x:row r="58" spans="1:11" outlineLevel="3">
       <x:c r="B58" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C58" s="41" t="n">
         <x:v>1212</x:v>
@@ -2410,7 +2405,7 @@
     </x:row>
     <x:row r="59" spans="1:11" outlineLevel="3">
       <x:c r="B59" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C59" s="41" t="n">
         <x:v>1091</x:v>
@@ -2434,7 +2429,7 @@
     </x:row>
     <x:row r="60" spans="1:11" outlineLevel="3">
       <x:c r="B60" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C60" s="41" t="n">
         <x:v>1261</x:v>
@@ -2458,7 +2453,7 @@
     </x:row>
     <x:row r="61" spans="1:11" outlineLevel="3">
       <x:c r="B61" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C61" s="41" t="n">
         <x:v>1012</x:v>
@@ -2482,7 +2477,7 @@
     </x:row>
     <x:row r="62" spans="1:11" outlineLevel="3">
       <x:c r="B62" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C62" s="41" t="n">
         <x:v>1161</x:v>
@@ -2508,7 +2503,7 @@
       <x:c r="B63" s="34" t="s"/>
       <x:c r="C63" s="34" t="s"/>
       <x:c r="D63" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E63" s="36" t="s"/>
       <x:c r="F63" s="37" t="s"/>
@@ -2520,13 +2515,13 @@
     </x:row>
     <x:row r="64" spans="1:11" outlineLevel="3">
       <x:c r="B64" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C64" s="41" t="n">
         <x:v>1168</x:v>
       </x:c>
       <x:c r="D64" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E64" s="42">
         <x:v>34519</x:v>
@@ -2548,7 +2543,7 @@
       <x:c r="B65" s="34" t="s"/>
       <x:c r="C65" s="34" t="s"/>
       <x:c r="D65" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E65" s="36" t="s"/>
       <x:c r="F65" s="37" t="s"/>
@@ -2560,13 +2555,13 @@
     </x:row>
     <x:row r="66" spans="1:11" outlineLevel="3">
       <x:c r="B66" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C66" s="41" t="n">
         <x:v>1148</x:v>
       </x:c>
       <x:c r="D66" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E66" s="42">
         <x:v>34396</x:v>
@@ -2586,7 +2581,7 @@
     </x:row>
     <x:row r="67" spans="1:11" outlineLevel="1">
       <x:c r="B67" s="34" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C67" s="34" t="s"/>
       <x:c r="D67" s="35" t="s"/>
@@ -2602,7 +2597,7 @@
       <x:c r="B68" s="34" t="s"/>
       <x:c r="C68" s="34" t="s"/>
       <x:c r="D68" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E68" s="36" t="s"/>
       <x:c r="F68" s="37" t="s"/>
@@ -2614,13 +2609,13 @@
     </x:row>
     <x:row r="69" spans="1:11" outlineLevel="3">
       <x:c r="B69" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C69" s="41" t="n">
         <x:v>1018</x:v>
       </x:c>
       <x:c r="D69" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E69" s="42">
         <x:v>32313</x:v>
@@ -2640,7 +2635,7 @@
     </x:row>
     <x:row r="70" spans="1:11" outlineLevel="3">
       <x:c r="B70" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C70" s="41" t="n">
         <x:v>1118</x:v>
@@ -2666,7 +2661,7 @@
       <x:c r="B71" s="34" t="s"/>
       <x:c r="C71" s="34" t="s"/>
       <x:c r="D71" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E71" s="36" t="s"/>
       <x:c r="F71" s="37" t="s"/>
@@ -2678,13 +2673,13 @@
     </x:row>
     <x:row r="72" spans="1:11" outlineLevel="3">
       <x:c r="B72" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C72" s="41" t="n">
         <x:v>1162</x:v>
       </x:c>
       <x:c r="D72" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E72" s="42">
         <x:v>34494</x:v>
@@ -2704,7 +2699,7 @@
     </x:row>
     <x:row r="73" spans="1:11" outlineLevel="3">
       <x:c r="B73" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C73" s="41" t="n">
         <x:v>1031</x:v>
@@ -2728,7 +2723,7 @@
     </x:row>
     <x:row r="74" spans="1:11" outlineLevel="3">
       <x:c r="B74" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C74" s="41" t="n">
         <x:v>1064</x:v>
@@ -2752,7 +2747,7 @@
     </x:row>
     <x:row r="75" spans="1:11" outlineLevel="3">
       <x:c r="B75" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C75" s="41" t="n">
         <x:v>1131</x:v>
@@ -2776,7 +2771,7 @@
     </x:row>
     <x:row r="76" spans="1:11" outlineLevel="3">
       <x:c r="B76" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C76" s="41" t="n">
         <x:v>1058</x:v>
@@ -2800,7 +2795,7 @@
     </x:row>
     <x:row r="77" spans="1:11" outlineLevel="3">
       <x:c r="B77" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C77" s="41" t="n">
         <x:v>1062</x:v>
@@ -2824,7 +2819,7 @@
     </x:row>
     <x:row r="78" spans="1:11" outlineLevel="1">
       <x:c r="B78" s="34" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C78" s="34" t="s"/>
       <x:c r="D78" s="35" t="s"/>
@@ -2840,7 +2835,7 @@
       <x:c r="B79" s="34" t="s"/>
       <x:c r="C79" s="34" t="s"/>
       <x:c r="D79" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E79" s="36" t="s"/>
       <x:c r="F79" s="37" t="s"/>
@@ -2852,13 +2847,13 @@
     </x:row>
     <x:row r="80" spans="1:11" outlineLevel="3">
       <x:c r="B80" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C80" s="41" t="n">
         <x:v>1066</x:v>
       </x:c>
       <x:c r="D80" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E80" s="42">
         <x:v>32594</x:v>
@@ -2878,7 +2873,7 @@
     </x:row>
     <x:row r="81" spans="1:11" outlineLevel="3">
       <x:c r="B81" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C81" s="41" t="n">
         <x:v>1205</x:v>
@@ -2902,7 +2897,7 @@
     </x:row>
     <x:row r="82" spans="1:11" outlineLevel="3">
       <x:c r="B82" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C82" s="41" t="n">
         <x:v>1166</x:v>
@@ -2926,7 +2921,7 @@
     </x:row>
     <x:row r="83" spans="1:11" outlineLevel="1">
       <x:c r="B83" s="34" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C83" s="34" t="s"/>
       <x:c r="D83" s="35" t="s"/>
@@ -2942,7 +2937,7 @@
       <x:c r="B84" s="34" t="s"/>
       <x:c r="C84" s="34" t="s"/>
       <x:c r="D84" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E84" s="36" t="s"/>
       <x:c r="F84" s="37" t="s"/>
@@ -2954,13 +2949,13 @@
     </x:row>
     <x:row r="85" spans="1:11" outlineLevel="3">
       <x:c r="B85" s="40" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C85" s="41" t="n">
         <x:v>1104</x:v>
       </x:c>
       <x:c r="D85" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E85" s="42">
         <x:v>33803</x:v>
@@ -2982,7 +2977,7 @@
       <x:c r="B86" s="34" t="s"/>
       <x:c r="C86" s="34" t="s"/>
       <x:c r="D86" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E86" s="36" t="s"/>
       <x:c r="F86" s="37" t="s"/>
@@ -2994,13 +2989,13 @@
     </x:row>
     <x:row r="87" spans="1:11" outlineLevel="3">
       <x:c r="B87" s="40" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C87" s="41" t="n">
         <x:v>1292</x:v>
       </x:c>
       <x:c r="D87" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E87" s="42">
         <x:v>34700</x:v>
@@ -3020,7 +3015,7 @@
     </x:row>
     <x:row r="88" spans="1:11" outlineLevel="1">
       <x:c r="B88" s="34" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C88" s="34" t="s"/>
       <x:c r="D88" s="35" t="s"/>
@@ -3036,7 +3031,7 @@
       <x:c r="B89" s="34" t="s"/>
       <x:c r="C89" s="34" t="s"/>
       <x:c r="D89" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E89" s="36" t="s"/>
       <x:c r="F89" s="37" t="s"/>
@@ -3048,13 +3043,13 @@
     </x:row>
     <x:row r="90" spans="1:11" outlineLevel="3">
       <x:c r="B90" s="40" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C90" s="41" t="n">
         <x:v>1134</x:v>
       </x:c>
       <x:c r="D90" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E90" s="42">
         <x:v>34287</x:v>
@@ -3074,7 +3069,7 @@
     </x:row>
     <x:row r="91" spans="1:11" outlineLevel="1">
       <x:c r="B91" s="34" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C91" s="34" t="s"/>
       <x:c r="D91" s="35" t="s"/>
@@ -3090,7 +3085,7 @@
       <x:c r="B92" s="34" t="s"/>
       <x:c r="C92" s="34" t="s"/>
       <x:c r="D92" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E92" s="36" t="s"/>
       <x:c r="F92" s="37" t="s"/>
@@ -3102,13 +3097,13 @@
     </x:row>
     <x:row r="93" spans="1:11" outlineLevel="3">
       <x:c r="B93" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C93" s="41" t="n">
         <x:v>1004</x:v>
       </x:c>
       <x:c r="D93" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E93" s="42">
         <x:v>32251</x:v>
@@ -3130,7 +3125,7 @@
       <x:c r="B94" s="34" t="s"/>
       <x:c r="C94" s="34" t="s"/>
       <x:c r="D94" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E94" s="36" t="s"/>
       <x:c r="F94" s="37" t="s"/>
@@ -3142,13 +3137,13 @@
     </x:row>
     <x:row r="95" spans="1:11" outlineLevel="3">
       <x:c r="B95" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C95" s="41" t="n">
         <x:v>1020</x:v>
       </x:c>
       <x:c r="D95" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E95" s="42">
         <x:v>32319</x:v>
@@ -3168,7 +3163,7 @@
     </x:row>
     <x:row r="96" spans="1:11" outlineLevel="3">
       <x:c r="B96" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C96" s="41" t="n">
         <x:v>1120</x:v>
@@ -3194,7 +3189,7 @@
       <x:c r="B97" s="34" t="s"/>
       <x:c r="C97" s="34" t="s"/>
       <x:c r="D97" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E97" s="36" t="s"/>
       <x:c r="F97" s="37" t="s"/>
@@ -3206,13 +3201,13 @@
     </x:row>
     <x:row r="98" spans="1:11" outlineLevel="3">
       <x:c r="B98" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C98" s="41" t="n">
         <x:v>1295</x:v>
       </x:c>
       <x:c r="D98" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E98" s="42">
         <x:v>34705</x:v>
@@ -3232,7 +3227,7 @@
     </x:row>
     <x:row r="99" spans="1:11" outlineLevel="3">
       <x:c r="B99" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C99" s="41" t="n">
         <x:v>1095</x:v>
@@ -3256,7 +3251,7 @@
     </x:row>
     <x:row r="100" spans="1:11" outlineLevel="1">
       <x:c r="B100" s="34" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C100" s="34" t="s"/>
       <x:c r="D100" s="35" t="s"/>
@@ -3272,7 +3267,7 @@
       <x:c r="B101" s="34" t="s"/>
       <x:c r="C101" s="34" t="s"/>
       <x:c r="D101" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E101" s="36" t="s"/>
       <x:c r="F101" s="37" t="s"/>
@@ -3284,13 +3279,13 @@
     </x:row>
     <x:row r="102" spans="1:11" outlineLevel="3">
       <x:c r="B102" s="40" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C102" s="41" t="n">
         <x:v>1260</x:v>
       </x:c>
       <x:c r="D102" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E102" s="42">
         <x:v>34678</x:v>
@@ -3312,7 +3307,7 @@
       <x:c r="B103" s="34" t="s"/>
       <x:c r="C103" s="34" t="s"/>
       <x:c r="D103" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E103" s="36" t="s"/>
       <x:c r="F103" s="37" t="s"/>
@@ -3324,13 +3319,13 @@
     </x:row>
     <x:row r="104" spans="1:11" outlineLevel="3">
       <x:c r="B104" s="40" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C104" s="41" t="n">
         <x:v>1078</x:v>
       </x:c>
       <x:c r="D104" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E104" s="42">
         <x:v>32630</x:v>
@@ -3350,7 +3345,7 @@
     </x:row>
     <x:row r="105" spans="1:11" outlineLevel="1">
       <x:c r="B105" s="34" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C105" s="34" t="s"/>
       <x:c r="D105" s="35" t="s"/>
@@ -3366,7 +3361,7 @@
       <x:c r="B106" s="34" t="s"/>
       <x:c r="C106" s="34" t="s"/>
       <x:c r="D106" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E106" s="36" t="s"/>
       <x:c r="F106" s="37" t="s"/>
@@ -3378,13 +3373,13 @@
     </x:row>
     <x:row r="107" spans="1:11" outlineLevel="3">
       <x:c r="B107" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C107" s="41" t="n">
         <x:v>1046</x:v>
       </x:c>
       <x:c r="D107" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E107" s="42">
         <x:v>32460</x:v>
@@ -3404,7 +3399,7 @@
     </x:row>
     <x:row r="108" spans="1:11" outlineLevel="3">
       <x:c r="B108" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C108" s="41" t="n">
         <x:v>1146</x:v>
@@ -3430,7 +3425,7 @@
       <x:c r="B109" s="34" t="s"/>
       <x:c r="C109" s="34" t="s"/>
       <x:c r="D109" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E109" s="36" t="s"/>
       <x:c r="F109" s="37" t="s"/>
@@ -3442,13 +3437,13 @@
     </x:row>
     <x:row r="110" spans="1:11" outlineLevel="3">
       <x:c r="B110" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C110" s="41" t="n">
         <x:v>1098</x:v>
       </x:c>
       <x:c r="D110" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E110" s="42">
         <x:v>32673</x:v>
@@ -3468,7 +3463,7 @@
     </x:row>
     <x:row r="111" spans="1:11" outlineLevel="3">
       <x:c r="B111" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C111" s="41" t="n">
         <x:v>1298</x:v>
@@ -3492,7 +3487,7 @@
     </x:row>
     <x:row r="112" spans="1:11" outlineLevel="3">
       <x:c r="B112" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C112" s="41" t="n">
         <x:v>1198</x:v>
@@ -3516,7 +3511,7 @@
     </x:row>
     <x:row r="113" spans="1:11" outlineLevel="1">
       <x:c r="B113" s="34" t="s">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C113" s="34" t="s"/>
       <x:c r="D113" s="35" t="s"/>
@@ -3532,7 +3527,7 @@
       <x:c r="B114" s="34" t="s"/>
       <x:c r="C114" s="34" t="s"/>
       <x:c r="D114" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E114" s="36" t="s"/>
       <x:c r="F114" s="37" t="s"/>
@@ -3544,13 +3539,13 @@
     </x:row>
     <x:row r="115" spans="1:11" outlineLevel="3">
       <x:c r="B115" s="40" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C115" s="41" t="n">
         <x:v>1130</x:v>
       </x:c>
       <x:c r="D115" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E115" s="42">
         <x:v>34268</x:v>
@@ -3570,7 +3565,7 @@
     </x:row>
     <x:row r="116" spans="1:11" outlineLevel="1">
       <x:c r="B116" s="34" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C116" s="34" t="s"/>
       <x:c r="D116" s="35" t="s"/>
@@ -3586,7 +3581,7 @@
       <x:c r="B117" s="34" t="s"/>
       <x:c r="C117" s="34" t="s"/>
       <x:c r="D117" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E117" s="36" t="s"/>
       <x:c r="F117" s="37" t="s"/>
@@ -3598,13 +3593,13 @@
     </x:row>
     <x:row r="118" spans="1:11" outlineLevel="3">
       <x:c r="B118" s="40" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C118" s="41" t="n">
         <x:v>1048</x:v>
       </x:c>
       <x:c r="D118" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E118" s="42">
         <x:v>32480</x:v>
@@ -3624,7 +3619,7 @@
     </x:row>
     <x:row r="119" spans="1:11" outlineLevel="3">
       <x:c r="B119" s="40" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C119" s="41" t="n">
         <x:v>1054</x:v>
@@ -3648,7 +3643,7 @@
     </x:row>
     <x:row r="120" spans="1:11" outlineLevel="1">
       <x:c r="B120" s="34" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C120" s="34" t="s"/>
       <x:c r="D120" s="35" t="s"/>
@@ -3664,7 +3659,7 @@
       <x:c r="B121" s="34" t="s"/>
       <x:c r="C121" s="34" t="s"/>
       <x:c r="D121" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E121" s="36" t="s"/>
       <x:c r="F121" s="37" t="s"/>
@@ -3676,13 +3671,13 @@
     </x:row>
     <x:row r="122" spans="1:11" outlineLevel="3">
       <x:c r="B122" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C122" s="41" t="n">
         <x:v>1086</x:v>
       </x:c>
       <x:c r="D122" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E122" s="42">
         <x:v>32647</x:v>
@@ -3704,7 +3699,7 @@
       <x:c r="B123" s="34" t="s"/>
       <x:c r="C123" s="34" t="s"/>
       <x:c r="D123" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E123" s="36" t="s"/>
       <x:c r="F123" s="37" t="s"/>
@@ -3716,13 +3711,13 @@
     </x:row>
     <x:row r="124" spans="1:11" outlineLevel="3">
       <x:c r="B124" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C124" s="41" t="n">
         <x:v>1209</x:v>
       </x:c>
       <x:c r="D124" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E124" s="42">
         <x:v>34650</x:v>
@@ -3742,7 +3737,7 @@
     </x:row>
     <x:row r="125" spans="1:11" outlineLevel="3">
       <x:c r="B125" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C125" s="41" t="n">
         <x:v>1109</x:v>
@@ -3766,7 +3761,7 @@
     </x:row>
     <x:row r="126" spans="1:11" outlineLevel="3">
       <x:c r="B126" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C126" s="41" t="n">
         <x:v>1009</x:v>
@@ -3792,7 +3787,7 @@
       <x:c r="B127" s="34" t="s"/>
       <x:c r="C127" s="34" t="s"/>
       <x:c r="D127" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E127" s="36" t="s"/>
       <x:c r="F127" s="37" t="s"/>
@@ -3804,13 +3799,13 @@
     </x:row>
     <x:row r="128" spans="1:11" outlineLevel="3">
       <x:c r="B128" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C128" s="41" t="n">
         <x:v>1090</x:v>
       </x:c>
       <x:c r="D128" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E128" s="42">
         <x:v>32654</x:v>
@@ -3832,7 +3827,7 @@
       <x:c r="B129" s="34" t="s"/>
       <x:c r="C129" s="34" t="s"/>
       <x:c r="D129" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E129" s="36" t="s"/>
       <x:c r="F129" s="37" t="s"/>
@@ -3844,13 +3839,13 @@
     </x:row>
     <x:row r="130" spans="1:11" outlineLevel="3">
       <x:c r="B130" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C130" s="41" t="n">
         <x:v>1056</x:v>
       </x:c>
       <x:c r="D130" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E130" s="42">
         <x:v>32548</x:v>
@@ -3870,7 +3865,7 @@
     </x:row>
     <x:row r="131" spans="1:11" outlineLevel="3">
       <x:c r="B131" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C131" s="41" t="n">
         <x:v>1197</x:v>
@@ -3894,7 +3889,7 @@
     </x:row>
     <x:row r="132" spans="1:11" outlineLevel="3">
       <x:c r="B132" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C132" s="41" t="n">
         <x:v>1156</x:v>
@@ -3920,7 +3915,7 @@
       <x:c r="B133" s="34" t="s"/>
       <x:c r="C133" s="34" t="s"/>
       <x:c r="D133" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E133" s="36" t="s"/>
       <x:c r="F133" s="37" t="s"/>
@@ -3932,13 +3927,13 @@
     </x:row>
     <x:row r="134" spans="1:11" outlineLevel="3">
       <x:c r="B134" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C134" s="41" t="n">
         <x:v>1165</x:v>
       </x:c>
       <x:c r="D134" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E134" s="42">
         <x:v>34511</x:v>
@@ -3958,7 +3953,7 @@
     </x:row>
     <x:row r="135" spans="1:11" outlineLevel="1">
       <x:c r="B135" s="34" t="s">
-        <x:v>60</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C135" s="34" t="s"/>
       <x:c r="D135" s="35" t="s"/>
@@ -3974,7 +3969,7 @@
       <x:c r="B136" s="34" t="s"/>
       <x:c r="C136" s="34" t="s"/>
       <x:c r="D136" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E136" s="36" t="s"/>
       <x:c r="F136" s="37" t="s"/>
@@ -3986,13 +3981,13 @@
     </x:row>
     <x:row r="137" spans="1:11" outlineLevel="3">
       <x:c r="B137" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C137" s="41" t="n">
         <x:v>1133</x:v>
       </x:c>
       <x:c r="D137" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E137" s="42">
         <x:v>34275</x:v>
@@ -4014,7 +4009,7 @@
       <x:c r="B138" s="34" t="s"/>
       <x:c r="C138" s="34" t="s"/>
       <x:c r="D138" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E138" s="36" t="s"/>
       <x:c r="F138" s="37" t="s"/>
@@ -4026,13 +4021,13 @@
     </x:row>
     <x:row r="139" spans="1:11" outlineLevel="3">
       <x:c r="B139" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C139" s="41" t="n">
         <x:v>1024</x:v>
       </x:c>
       <x:c r="D139" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E139" s="42">
         <x:v>32327</x:v>
@@ -4054,7 +4049,7 @@
       <x:c r="B140" s="34" t="s"/>
       <x:c r="C140" s="34" t="s"/>
       <x:c r="D140" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E140" s="36" t="s"/>
       <x:c r="F140" s="37" t="s"/>
@@ -4066,13 +4061,13 @@
     </x:row>
     <x:row r="141" spans="1:11" outlineLevel="3">
       <x:c r="B141" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C141" s="41" t="n">
         <x:v>1089</x:v>
       </x:c>
       <x:c r="D141" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E141" s="42">
         <x:v>32651</x:v>
@@ -4092,7 +4087,7 @@
     </x:row>
     <x:row r="142" spans="1:11" outlineLevel="1">
       <x:c r="B142" s="34" t="s">
-        <x:v>62</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C142" s="34" t="s"/>
       <x:c r="D142" s="35" t="s"/>
@@ -4108,7 +4103,7 @@
       <x:c r="B143" s="34" t="s"/>
       <x:c r="C143" s="34" t="s"/>
       <x:c r="D143" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E143" s="36" t="s"/>
       <x:c r="F143" s="37" t="s"/>
@@ -4120,13 +4115,13 @@
     </x:row>
     <x:row r="144" spans="1:11" outlineLevel="3">
       <x:c r="B144" s="40" t="s">
-        <x:v>63</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C144" s="41" t="n">
         <x:v>1019</x:v>
       </x:c>
       <x:c r="D144" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E144" s="42">
         <x:v>32319</x:v>
@@ -4146,7 +4141,7 @@
     </x:row>
     <x:row r="145" spans="1:11" outlineLevel="1">
       <x:c r="B145" s="34" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C145" s="34" t="s"/>
       <x:c r="D145" s="35" t="s"/>
@@ -4162,7 +4157,7 @@
       <x:c r="B146" s="34" t="s"/>
       <x:c r="C146" s="34" t="s"/>
       <x:c r="D146" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E146" s="36" t="s"/>
       <x:c r="F146" s="37" t="s"/>
@@ -4174,13 +4169,13 @@
     </x:row>
     <x:row r="147" spans="1:11" outlineLevel="3">
       <x:c r="B147" s="40" t="s">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C147" s="41" t="n">
         <x:v>1069</x:v>
       </x:c>
       <x:c r="D147" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E147" s="42">
         <x:v>32604</x:v>
@@ -4200,7 +4195,7 @@
     </x:row>
     <x:row r="148" spans="1:11" outlineLevel="1">
       <x:c r="B148" s="34" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C148" s="34" t="s"/>
       <x:c r="D148" s="35" t="s"/>
@@ -4216,7 +4211,7 @@
       <x:c r="B149" s="34" t="s"/>
       <x:c r="C149" s="34" t="s"/>
       <x:c r="D149" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E149" s="36" t="s"/>
       <x:c r="F149" s="37" t="s"/>
@@ -4228,13 +4223,13 @@
     </x:row>
     <x:row r="150" spans="1:11" outlineLevel="3">
       <x:c r="B150" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C150" s="41" t="n">
         <x:v>1081</x:v>
       </x:c>
       <x:c r="D150" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E150" s="42">
         <x:v>32636</x:v>
@@ -4256,7 +4251,7 @@
       <x:c r="B151" s="34" t="s"/>
       <x:c r="C151" s="34" t="s"/>
       <x:c r="D151" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E151" s="36" t="s"/>
       <x:c r="F151" s="37" t="s"/>
@@ -4268,13 +4263,13 @@
     </x:row>
     <x:row r="152" spans="1:11" outlineLevel="3">
       <x:c r="B152" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C152" s="41" t="n">
         <x:v>1103</x:v>
       </x:c>
       <x:c r="D152" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E152" s="42">
         <x:v>33798</x:v>
@@ -4294,7 +4289,7 @@
     </x:row>
     <x:row r="153" spans="1:11" outlineLevel="3">
       <x:c r="B153" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C153" s="41" t="n">
         <x:v>1063</x:v>
@@ -4318,7 +4313,7 @@
     </x:row>
     <x:row r="154" spans="1:11" outlineLevel="1">
       <x:c r="B154" s="34" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C154" s="34" t="s"/>
       <x:c r="D154" s="35" t="s"/>
@@ -4334,7 +4329,7 @@
       <x:c r="B155" s="34" t="s"/>
       <x:c r="C155" s="34" t="s"/>
       <x:c r="D155" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E155" s="36" t="s"/>
       <x:c r="F155" s="37" t="s"/>
@@ -4346,13 +4341,13 @@
     </x:row>
     <x:row r="156" spans="1:11" outlineLevel="3">
       <x:c r="B156" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C156" s="41" t="n">
         <x:v>1016</x:v>
       </x:c>
       <x:c r="D156" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E156" s="42">
         <x:v>32297</x:v>
@@ -4372,7 +4367,7 @@
     </x:row>
     <x:row r="157" spans="1:11" outlineLevel="3">
       <x:c r="B157" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C157" s="41" t="n">
         <x:v>1116</x:v>
@@ -4398,7 +4393,7 @@
       <x:c r="B158" s="34" t="s"/>
       <x:c r="C158" s="34" t="s"/>
       <x:c r="D158" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E158" s="36" t="s"/>
       <x:c r="F158" s="37" t="s"/>
@@ -4410,13 +4405,13 @@
     </x:row>
     <x:row r="159" spans="1:11" outlineLevel="3">
       <x:c r="B159" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C159" s="41" t="n">
         <x:v>1084</x:v>
       </x:c>
       <x:c r="D159" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E159" s="42">
         <x:v>32640</x:v>
@@ -4438,7 +4433,7 @@
       <x:c r="B160" s="34" t="s"/>
       <x:c r="C160" s="34" t="s"/>
       <x:c r="D160" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E160" s="36" t="s"/>
       <x:c r="F160" s="37" t="s"/>
@@ -4450,13 +4445,13 @@
     </x:row>
     <x:row r="161" spans="1:11" outlineLevel="3">
       <x:c r="B161" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C161" s="41" t="n">
         <x:v>1034</x:v>
       </x:c>
       <x:c r="D161" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E161" s="42">
         <x:v>32369</x:v>
@@ -4478,7 +4473,7 @@
       <x:c r="B162" s="34" t="s"/>
       <x:c r="C162" s="34" t="s"/>
       <x:c r="D162" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E162" s="36" t="s"/>
       <x:c r="F162" s="37" t="s"/>
@@ -4490,13 +4485,13 @@
     </x:row>
     <x:row r="163" spans="1:11" outlineLevel="3">
       <x:c r="B163" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C163" s="41" t="n">
         <x:v>1093</x:v>
       </x:c>
       <x:c r="D163" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E163" s="42">
         <x:v>32661</x:v>
@@ -4516,7 +4511,7 @@
     </x:row>
     <x:row r="164" spans="1:11" outlineLevel="1">
       <x:c r="B164" s="34" t="s">
-        <x:v>70</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C164" s="34" t="s"/>
       <x:c r="D164" s="35" t="s"/>
@@ -4532,7 +4527,7 @@
       <x:c r="B165" s="34" t="s"/>
       <x:c r="C165" s="34" t="s"/>
       <x:c r="D165" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E165" s="36" t="s"/>
       <x:c r="F165" s="37" t="s"/>
@@ -4544,13 +4539,13 @@
     </x:row>
     <x:row r="166" spans="1:11" outlineLevel="3">
       <x:c r="B166" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C166" s="41" t="n">
         <x:v>1015</x:v>
       </x:c>
       <x:c r="D166" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E166" s="42">
         <x:v>32289</x:v>
@@ -4570,7 +4565,7 @@
     </x:row>
     <x:row r="167" spans="1:11" outlineLevel="3">
       <x:c r="B167" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C167" s="41" t="n">
         <x:v>1315</x:v>
@@ -4594,7 +4589,7 @@
     </x:row>
     <x:row r="168" spans="1:11" outlineLevel="3">
       <x:c r="B168" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C168" s="41" t="n">
         <x:v>1215</x:v>
@@ -4620,7 +4615,7 @@
       <x:c r="B169" s="34" t="s"/>
       <x:c r="C169" s="34" t="s"/>
       <x:c r="D169" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E169" s="36" t="s"/>
       <x:c r="F169" s="37" t="s"/>
@@ -4632,13 +4627,13 @@
     </x:row>
     <x:row r="170" spans="1:11" outlineLevel="3">
       <x:c r="B170" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C170" s="41" t="n">
         <x:v>1128</x:v>
       </x:c>
       <x:c r="D170" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E170" s="42">
         <x:v>34250</x:v>
@@ -4658,7 +4653,7 @@
     </x:row>
     <x:row r="171" spans="1:11" outlineLevel="3">
       <x:c r="B171" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C171" s="41" t="n">
         <x:v>1028</x:v>
@@ -4682,7 +4677,7 @@
     </x:row>
     <x:row r="172" spans="1:11" outlineLevel="1">
       <x:c r="B172" s="34" t="s">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C172" s="34" t="s"/>
       <x:c r="D172" s="35" t="s"/>
@@ -4698,7 +4693,7 @@
       <x:c r="B173" s="34" t="s"/>
       <x:c r="C173" s="34" t="s"/>
       <x:c r="D173" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E173" s="36" t="s"/>
       <x:c r="F173" s="37" t="s"/>
@@ -4710,13 +4705,13 @@
     </x:row>
     <x:row r="174" spans="1:11" outlineLevel="3">
       <x:c r="B174" s="40" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C174" s="41" t="n">
         <x:v>1141</x:v>
       </x:c>
       <x:c r="D174" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E174" s="42">
         <x:v>34320</x:v>
@@ -4736,7 +4731,7 @@
     </x:row>
     <x:row r="175" spans="1:11" outlineLevel="3">
       <x:c r="B175" s="40" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C175" s="41" t="n">
         <x:v>1041</x:v>
@@ -4760,7 +4755,7 @@
     </x:row>
     <x:row r="176" spans="1:11" outlineLevel="1">
       <x:c r="B176" s="34" t="s">
-        <x:v>74</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C176" s="34" t="s"/>
       <x:c r="D176" s="35" t="s"/>
@@ -4776,7 +4771,7 @@
       <x:c r="B177" s="34" t="s"/>
       <x:c r="C177" s="34" t="s"/>
       <x:c r="D177" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E177" s="36" t="s"/>
       <x:c r="F177" s="37" t="s"/>
@@ -4788,13 +4783,13 @@
     </x:row>
     <x:row r="178" spans="1:11" outlineLevel="3">
       <x:c r="B178" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C178" s="41" t="n">
         <x:v>1023</x:v>
       </x:c>
       <x:c r="D178" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E178" s="42">
         <x:v>32326</x:v>
@@ -4814,7 +4809,7 @@
     </x:row>
     <x:row r="179" spans="1:11" outlineLevel="3">
       <x:c r="B179" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C179" s="41" t="n">
         <x:v>1123</x:v>
@@ -4840,7 +4835,7 @@
       <x:c r="B180" s="34" t="s"/>
       <x:c r="C180" s="34" t="s"/>
       <x:c r="D180" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E180" s="36" t="s"/>
       <x:c r="F180" s="37" t="s"/>
@@ -4852,13 +4847,13 @@
     </x:row>
     <x:row r="181" spans="1:11" outlineLevel="3">
       <x:c r="B181" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C181" s="41" t="n">
         <x:v>1269</x:v>
       </x:c>
       <x:c r="D181" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E181" s="42">
         <x:v>34684</x:v>
@@ -4878,7 +4873,7 @@
     </x:row>
     <x:row r="182" spans="1:11" outlineLevel="3">
       <x:c r="B182" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C182" s="41" t="n">
         <x:v>1169</x:v>
@@ -4904,7 +4899,7 @@
       <x:c r="B183" s="34" t="s"/>
       <x:c r="C183" s="34" t="s"/>
       <x:c r="D183" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E183" s="36" t="s"/>
       <x:c r="F183" s="37" t="s"/>
@@ -4916,13 +4911,13 @@
     </x:row>
     <x:row r="184" spans="1:11" outlineLevel="3">
       <x:c r="B184" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C184" s="41" t="n">
         <x:v>1076</x:v>
       </x:c>
       <x:c r="D184" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E184" s="42">
         <x:v>32624</x:v>
@@ -4942,7 +4937,7 @@
     </x:row>
     <x:row r="185" spans="1:11" outlineLevel="3">
       <x:c r="B185" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C185" s="41" t="n">
         <x:v>1176</x:v>
@@ -4966,7 +4961,7 @@
     </x:row>
     <x:row r="186" spans="1:11" outlineLevel="1">
       <x:c r="B186" s="34" t="s">
-        <x:v>76</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C186" s="34" t="s"/>
       <x:c r="D186" s="35" t="s"/>
@@ -4982,7 +4977,7 @@
       <x:c r="B187" s="34" t="s"/>
       <x:c r="C187" s="34" t="s"/>
       <x:c r="D187" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E187" s="36" t="s"/>
       <x:c r="F187" s="37" t="s"/>
@@ -4994,13 +4989,13 @@
     </x:row>
     <x:row r="188" spans="1:11" outlineLevel="3">
       <x:c r="B188" s="40" t="s">
-        <x:v>77</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C188" s="41" t="n">
         <x:v>1096</x:v>
       </x:c>
       <x:c r="D188" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E188" s="42">
         <x:v>32668</x:v>
@@ -5020,7 +5015,7 @@
     </x:row>
     <x:row r="189" spans="1:11" outlineLevel="3">
       <x:c r="B189" s="40" t="s">
-        <x:v>77</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C189" s="41" t="n">
         <x:v>1196</x:v>
@@ -5044,7 +5039,7 @@
     </x:row>
     <x:row r="190" spans="1:11" outlineLevel="1">
       <x:c r="B190" s="34" t="s">
-        <x:v>78</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C190" s="34" t="s"/>
       <x:c r="D190" s="35" t="s"/>
@@ -5060,7 +5055,7 @@
       <x:c r="B191" s="34" t="s"/>
       <x:c r="C191" s="34" t="s"/>
       <x:c r="D191" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E191" s="36" t="s"/>
       <x:c r="F191" s="37" t="s"/>
@@ -5072,13 +5067,13 @@
     </x:row>
     <x:row r="192" spans="1:11" outlineLevel="3">
       <x:c r="B192" s="40" t="s">
-        <x:v>79</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C192" s="41" t="n">
         <x:v>1158</x:v>
       </x:c>
       <x:c r="D192" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E192" s="42">
         <x:v>34476</x:v>
@@ -5098,7 +5093,7 @@
     </x:row>
     <x:row r="193" spans="1:11" outlineLevel="1">
       <x:c r="B193" s="34" t="s">
-        <x:v>80</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C193" s="34" t="s"/>
       <x:c r="D193" s="35" t="s"/>
@@ -5114,7 +5109,7 @@
       <x:c r="B194" s="34" t="s"/>
       <x:c r="C194" s="34" t="s"/>
       <x:c r="D194" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E194" s="36" t="s"/>
       <x:c r="F194" s="37" t="s"/>
@@ -5126,13 +5121,13 @@
     </x:row>
     <x:row r="195" spans="1:11" outlineLevel="3">
       <x:c r="B195" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C195" s="41" t="n">
         <x:v>1026</x:v>
       </x:c>
       <x:c r="D195" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E195" s="42">
         <x:v>32332</x:v>
@@ -5152,7 +5147,7 @@
     </x:row>
     <x:row r="196" spans="1:11" outlineLevel="3">
       <x:c r="B196" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C196" s="41" t="n">
         <x:v>1126</x:v>
@@ -5178,7 +5173,7 @@
       <x:c r="B197" s="34" t="s"/>
       <x:c r="C197" s="34" t="s"/>
       <x:c r="D197" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E197" s="36" t="s"/>
       <x:c r="F197" s="37" t="s"/>
@@ -5190,13 +5185,13 @@
     </x:row>
     <x:row r="198" spans="1:11" outlineLevel="3">
       <x:c r="B198" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C198" s="41" t="n">
         <x:v>1013</x:v>
       </x:c>
       <x:c r="D198" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E198" s="42">
         <x:v>32289</x:v>
@@ -5216,7 +5211,7 @@
     </x:row>
     <x:row r="199" spans="1:11" outlineLevel="3">
       <x:c r="B199" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C199" s="41" t="n">
         <x:v>1113</x:v>
@@ -5240,7 +5235,7 @@
     </x:row>
     <x:row r="200" spans="1:11" outlineLevel="1">
       <x:c r="B200" s="34" t="s">
-        <x:v>82</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C200" s="34" t="s"/>
       <x:c r="D200" s="35" t="s"/>
@@ -5256,7 +5251,7 @@
       <x:c r="B201" s="34" t="s"/>
       <x:c r="C201" s="34" t="s"/>
       <x:c r="D201" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E201" s="36" t="s"/>
       <x:c r="F201" s="37" t="s"/>
@@ -5268,13 +5263,13 @@
     </x:row>
     <x:row r="202" spans="1:11" outlineLevel="3">
       <x:c r="B202" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C202" s="41" t="n">
         <x:v>1860</x:v>
       </x:c>
       <x:c r="D202" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E202" s="42" t="s"/>
       <x:c r="F202" s="42">
@@ -5294,7 +5289,7 @@
       <x:c r="B203" s="34" t="s"/>
       <x:c r="C203" s="34" t="s"/>
       <x:c r="D203" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E203" s="36" t="s"/>
       <x:c r="F203" s="37" t="s"/>
@@ -5306,13 +5301,13 @@
     </x:row>
     <x:row r="204" spans="1:11" outlineLevel="3">
       <x:c r="B204" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C204" s="41" t="n">
         <x:v>1309</x:v>
       </x:c>
       <x:c r="D204" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E204" s="42">
         <x:v>34721</x:v>
@@ -5334,7 +5329,7 @@
       <x:c r="B205" s="34" t="s"/>
       <x:c r="C205" s="34" t="s"/>
       <x:c r="D205" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E205" s="36" t="s"/>
       <x:c r="F205" s="37" t="s"/>
@@ -5346,13 +5341,13 @@
     </x:row>
     <x:row r="206" spans="1:11" outlineLevel="3">
       <x:c r="B206" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C206" s="41" t="n">
         <x:v>1030</x:v>
       </x:c>
       <x:c r="D206" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E206" s="42">
         <x:v>32350</x:v>
@@ -5372,7 +5367,7 @@
     </x:row>
     <x:row r="207" spans="1:11" outlineLevel="3">
       <x:c r="B207" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C207" s="41" t="n">
         <x:v>1097</x:v>
@@ -5396,7 +5391,7 @@
     </x:row>
     <x:row r="208" spans="1:11" outlineLevel="1">
       <x:c r="B208" s="34" t="s">
-        <x:v>84</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C208" s="34" t="s"/>
       <x:c r="D208" s="35" t="s"/>
@@ -5412,7 +5407,7 @@
       <x:c r="B209" s="34" t="s"/>
       <x:c r="C209" s="34" t="s"/>
       <x:c r="D209" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E209" s="36" t="s"/>
       <x:c r="F209" s="37" t="s"/>
@@ -5424,13 +5419,13 @@
     </x:row>
     <x:row r="210" spans="1:11" outlineLevel="3">
       <x:c r="B210" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C210" s="41" t="n">
         <x:v>1082</x:v>
       </x:c>
       <x:c r="D210" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E210" s="42">
         <x:v>32638</x:v>
@@ -5452,7 +5447,7 @@
       <x:c r="B211" s="34" t="s"/>
       <x:c r="C211" s="34" t="s"/>
       <x:c r="D211" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E211" s="36" t="s"/>
       <x:c r="F211" s="37" t="s"/>
@@ -5464,13 +5459,13 @@
     </x:row>
     <x:row r="212" spans="1:11" outlineLevel="3">
       <x:c r="B212" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C212" s="41" t="n">
         <x:v>1010</x:v>
       </x:c>
       <x:c r="D212" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E212" s="42">
         <x:v>32275</x:v>
@@ -5492,7 +5487,7 @@
       <x:c r="B213" s="34" t="s"/>
       <x:c r="C213" s="34" t="s"/>
       <x:c r="D213" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E213" s="36" t="s"/>
       <x:c r="F213" s="37" t="s"/>
@@ -5504,13 +5499,13 @@
     </x:row>
     <x:row r="214" spans="1:11" outlineLevel="3">
       <x:c r="B214" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C214" s="41" t="n">
         <x:v>1170</x:v>
       </x:c>
       <x:c r="D214" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E214" s="42">
         <x:v>34523</x:v>
@@ -5530,7 +5525,7 @@
     </x:row>
     <x:row r="215" spans="1:11" outlineLevel="3">
       <x:c r="B215" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C215" s="41" t="n">
         <x:v>1077</x:v>
@@ -5554,7 +5549,7 @@
     </x:row>
     <x:row r="216" spans="1:11" outlineLevel="1">
       <x:c r="B216" s="34" t="s">
-        <x:v>86</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C216" s="34" t="s"/>
       <x:c r="D216" s="35" t="s"/>
@@ -5570,7 +5565,7 @@
       <x:c r="B217" s="34" t="s"/>
       <x:c r="C217" s="34" t="s"/>
       <x:c r="D217" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E217" s="36" t="s"/>
       <x:c r="F217" s="37" t="s"/>
@@ -5582,13 +5577,13 @@
     </x:row>
     <x:row r="218" spans="1:11" outlineLevel="3">
       <x:c r="B218" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C218" s="41" t="n">
         <x:v>1045</x:v>
       </x:c>
       <x:c r="D218" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E218" s="42">
         <x:v>32433</x:v>
@@ -5608,7 +5603,7 @@
     </x:row>
     <x:row r="219" spans="1:11" outlineLevel="3">
       <x:c r="B219" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C219" s="41" t="n">
         <x:v>1145</x:v>
@@ -5634,7 +5629,7 @@
       <x:c r="B220" s="34" t="s"/>
       <x:c r="C220" s="34" t="s"/>
       <x:c r="D220" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E220" s="36" t="s"/>
       <x:c r="F220" s="37" t="s"/>
@@ -5646,13 +5641,13 @@
     </x:row>
     <x:row r="221" spans="1:11" outlineLevel="3">
       <x:c r="B221" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C221" s="41" t="n">
         <x:v>1149</x:v>
       </x:c>
       <x:c r="D221" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E221" s="42">
         <x:v>34407</x:v>
@@ -5672,7 +5667,7 @@
     </x:row>
     <x:row r="222" spans="1:11" outlineLevel="3">
       <x:c r="B222" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C222" s="41" t="n">
         <x:v>1049</x:v>
@@ -5696,7 +5691,7 @@
     </x:row>
     <x:row r="223" spans="1:11" outlineLevel="1">
       <x:c r="B223" s="34" t="s">
-        <x:v>88</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C223" s="34" t="s"/>
       <x:c r="D223" s="35" t="s"/>
@@ -5712,7 +5707,7 @@
       <x:c r="B224" s="34" t="s"/>
       <x:c r="C224" s="34" t="s"/>
       <x:c r="D224" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E224" s="36" t="s"/>
       <x:c r="F224" s="37" t="s"/>
@@ -5724,13 +5719,13 @@
     </x:row>
     <x:row r="225" spans="1:11" outlineLevel="3">
       <x:c r="B225" s="40" t="s">
-        <x:v>89</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C225" s="41" t="n">
         <x:v>1092</x:v>
       </x:c>
       <x:c r="D225" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E225" s="42">
         <x:v>32660</x:v>
@@ -5750,7 +5745,7 @@
     </x:row>
     <x:row r="226" spans="1:11" outlineLevel="1">
       <x:c r="B226" s="34" t="s">
-        <x:v>90</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C226" s="34" t="s"/>
       <x:c r="D226" s="35" t="s"/>
@@ -5766,7 +5761,7 @@
       <x:c r="B227" s="34" t="s"/>
       <x:c r="C227" s="34" t="s"/>
       <x:c r="D227" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E227" s="36" t="s"/>
       <x:c r="F227" s="37" t="s"/>
@@ -5778,13 +5773,13 @@
     </x:row>
     <x:row r="228" spans="1:11" outlineLevel="3">
       <x:c r="B228" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C228" s="41" t="n">
         <x:v>1047</x:v>
       </x:c>
       <x:c r="D228" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E228" s="42">
         <x:v>32475</x:v>
@@ -5806,7 +5801,7 @@
       <x:c r="B229" s="34" t="s"/>
       <x:c r="C229" s="34" t="s"/>
       <x:c r="D229" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E229" s="36" t="s"/>
       <x:c r="F229" s="37" t="s"/>
@@ -5818,13 +5813,13 @@
     </x:row>
     <x:row r="230" spans="1:11" outlineLevel="3">
       <x:c r="B230" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C230" s="41" t="n">
         <x:v>1144</x:v>
       </x:c>
       <x:c r="D230" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E230" s="42">
         <x:v>34343</x:v>
@@ -5844,7 +5839,7 @@
     </x:row>
     <x:row r="231" spans="1:11" outlineLevel="3">
       <x:c r="B231" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C231" s="41" t="n">
         <x:v>1044</x:v>
@@ -5868,7 +5863,7 @@
     </x:row>
     <x:row r="232" spans="1:11" outlineLevel="1">
       <x:c r="B232" s="34" t="s">
-        <x:v>92</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C232" s="34" t="s"/>
       <x:c r="D232" s="35" t="s"/>
@@ -5884,7 +5879,7 @@
       <x:c r="B233" s="34" t="s"/>
       <x:c r="C233" s="34" t="s"/>
       <x:c r="D233" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E233" s="36" t="s"/>
       <x:c r="F233" s="37" t="s"/>
@@ -5896,13 +5891,13 @@
     </x:row>
     <x:row r="234" spans="1:11" outlineLevel="3">
       <x:c r="B234" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C234" s="41" t="n">
         <x:v>1025</x:v>
       </x:c>
       <x:c r="D234" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E234" s="42">
         <x:v>32328</x:v>
@@ -5922,7 +5917,7 @@
     </x:row>
     <x:row r="235" spans="1:11" outlineLevel="3">
       <x:c r="B235" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C235" s="41" t="n">
         <x:v>1125</x:v>
@@ -5948,7 +5943,7 @@
       <x:c r="B236" s="34" t="s"/>
       <x:c r="C236" s="34" t="s"/>
       <x:c r="D236" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E236" s="36" t="s"/>
       <x:c r="F236" s="37" t="s"/>
@@ -5960,13 +5955,13 @@
     </x:row>
     <x:row r="237" spans="1:11" outlineLevel="3">
       <x:c r="B237" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C237" s="41" t="n">
         <x:v>1008</x:v>
       </x:c>
       <x:c r="D237" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E237" s="42">
         <x:v>32267</x:v>
@@ -5986,7 +5981,7 @@
     </x:row>
     <x:row r="238" spans="1:11" outlineLevel="3">
       <x:c r="B238" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C238" s="41" t="n">
         <x:v>1139</x:v>
@@ -6010,7 +6005,7 @@
     </x:row>
     <x:row r="239" spans="1:11" outlineLevel="1">
       <x:c r="B239" s="34" t="s">
-        <x:v>94</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C239" s="34" t="s"/>
       <x:c r="D239" s="35" t="s"/>
@@ -6026,7 +6021,7 @@
       <x:c r="B240" s="34" t="s"/>
       <x:c r="C240" s="34" t="s"/>
       <x:c r="D240" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E240" s="36" t="s"/>
       <x:c r="F240" s="37" t="s"/>
@@ -6038,13 +6033,13 @@
     </x:row>
     <x:row r="241" spans="1:11" outlineLevel="3">
       <x:c r="B241" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C241" s="41" t="n">
         <x:v>1183</x:v>
       </x:c>
       <x:c r="D241" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E241" s="42">
         <x:v>34556</x:v>
@@ -6066,7 +6061,7 @@
       <x:c r="B242" s="34" t="s"/>
       <x:c r="C242" s="34" t="s"/>
       <x:c r="D242" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E242" s="36" t="s"/>
       <x:c r="F242" s="37" t="s"/>
@@ -6078,13 +6073,13 @@
     </x:row>
     <x:row r="243" spans="1:11" outlineLevel="3">
       <x:c r="B243" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C243" s="41" t="n">
         <x:v>1112</x:v>
       </x:c>
       <x:c r="D243" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E243" s="42">
         <x:v>33971</x:v>
@@ -6106,7 +6101,7 @@
       <x:c r="B244" s="34" t="s"/>
       <x:c r="C244" s="34" t="s"/>
       <x:c r="D244" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E244" s="36" t="s"/>
       <x:c r="F244" s="37" t="s"/>
@@ -6118,13 +6113,13 @@
     </x:row>
     <x:row r="245" spans="1:11" outlineLevel="3">
       <x:c r="B245" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C245" s="41" t="n">
         <x:v>1068</x:v>
       </x:c>
       <x:c r="D245" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E245" s="42">
         <x:v>32602</x:v>
@@ -6144,7 +6139,7 @@
     </x:row>
     <x:row r="246" spans="1:11" outlineLevel="1">
       <x:c r="B246" s="34" t="s">
-        <x:v>96</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C246" s="34" t="s"/>
       <x:c r="D246" s="35" t="s"/>
@@ -6160,7 +6155,7 @@
       <x:c r="B247" s="34" t="s"/>
       <x:c r="C247" s="34" t="s"/>
       <x:c r="D247" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E247" s="36" t="s"/>
       <x:c r="F247" s="37" t="s"/>
@@ -6172,13 +6167,13 @@
     </x:row>
     <x:row r="248" spans="1:11" outlineLevel="3">
       <x:c r="B248" s="40" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C248" s="41" t="n">
         <x:v>1043</x:v>
       </x:c>
       <x:c r="D248" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E248" s="42">
         <x:v>32417</x:v>
@@ -6198,7 +6193,7 @@
     </x:row>
     <x:row r="249" spans="1:11" outlineLevel="3">
       <x:c r="B249" s="40" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C249" s="41" t="n">
         <x:v>1143</x:v>
@@ -6222,7 +6217,7 @@
     </x:row>
     <x:row r="250" spans="1:11" outlineLevel="1">
       <x:c r="B250" s="34" t="s">
-        <x:v>98</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C250" s="34" t="s"/>
       <x:c r="D250" s="35" t="s"/>
@@ -6238,7 +6233,7 @@
       <x:c r="B251" s="34" t="s"/>
       <x:c r="C251" s="34" t="s"/>
       <x:c r="D251" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E251" s="36" t="s"/>
       <x:c r="F251" s="37" t="s"/>
@@ -6250,13 +6245,13 @@
     </x:row>
     <x:row r="252" spans="1:11" outlineLevel="3">
       <x:c r="B252" s="40" t="s">
-        <x:v>99</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C252" s="41" t="n">
         <x:v>1201</x:v>
       </x:c>
       <x:c r="D252" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E252" s="42">
         <x:v>34611</x:v>
@@ -6276,7 +6271,7 @@
     </x:row>
     <x:row r="253" spans="1:11" outlineLevel="1">
       <x:c r="B253" s="34" t="s">
-        <x:v>100</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C253" s="34" t="s"/>
       <x:c r="D253" s="35" t="s"/>
@@ -6292,7 +6287,7 @@
       <x:c r="B254" s="34" t="s"/>
       <x:c r="C254" s="34" t="s"/>
       <x:c r="D254" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E254" s="36" t="s"/>
       <x:c r="F254" s="37" t="s"/>
@@ -6304,13 +6299,13 @@
     </x:row>
     <x:row r="255" spans="1:11" outlineLevel="3">
       <x:c r="B255" s="40" t="s">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C255" s="41" t="n">
         <x:v>1199</x:v>
       </x:c>
       <x:c r="D255" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E255" s="42">
         <x:v>34593</x:v>
@@ -6332,7 +6327,7 @@
       <x:c r="B256" s="34" t="s"/>
       <x:c r="C256" s="34" t="s"/>
       <x:c r="D256" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E256" s="36" t="s"/>
       <x:c r="F256" s="37" t="s"/>
@@ -6344,13 +6339,13 @@
     </x:row>
     <x:row r="257" spans="1:11" outlineLevel="3">
       <x:c r="B257" s="40" t="s">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C257" s="41" t="n">
         <x:v>1094</x:v>
       </x:c>
       <x:c r="D257" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E257" s="42">
         <x:v>32663</x:v>
@@ -6370,7 +6365,7 @@
     </x:row>
     <x:row r="258" spans="1:11" outlineLevel="1">
       <x:c r="B258" s="34" t="s">
-        <x:v>102</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C258" s="34" t="s"/>
       <x:c r="D258" s="35" t="s"/>
@@ -6386,7 +6381,7 @@
       <x:c r="B259" s="34" t="s"/>
       <x:c r="C259" s="34" t="s"/>
       <x:c r="D259" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E259" s="36" t="s"/>
       <x:c r="F259" s="37" t="s"/>
@@ -6398,13 +6393,13 @@
     </x:row>
     <x:row r="260" spans="1:11" outlineLevel="3">
       <x:c r="B260" s="40" t="s">
-        <x:v>103</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C260" s="41" t="n">
         <x:v>1175</x:v>
       </x:c>
       <x:c r="D260" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E260" s="42">
         <x:v>34537</x:v>
@@ -6424,7 +6419,7 @@
     </x:row>
     <x:row r="261" spans="1:11" outlineLevel="1">
       <x:c r="B261" s="34" t="s">
-        <x:v>104</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C261" s="34" t="s"/>
       <x:c r="D261" s="35" t="s"/>
@@ -6440,7 +6435,7 @@
       <x:c r="B262" s="34" t="s"/>
       <x:c r="C262" s="34" t="s"/>
       <x:c r="D262" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E262" s="36" t="s"/>
       <x:c r="F262" s="37" t="s"/>
@@ -6452,13 +6447,13 @@
     </x:row>
     <x:row r="263" spans="1:11" outlineLevel="3">
       <x:c r="B263" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C263" s="41" t="n">
         <x:v>1132</x:v>
       </x:c>
       <x:c r="D263" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E263" s="42">
         <x:v>34274</x:v>
@@ -6478,7 +6473,7 @@
     </x:row>
     <x:row r="264" spans="1:11" outlineLevel="3">
       <x:c r="B264" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C264" s="41" t="n">
         <x:v>1221</x:v>
@@ -6502,7 +6497,7 @@
     </x:row>
     <x:row r="265" spans="1:11" outlineLevel="3">
       <x:c r="B265" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C265" s="41" t="n">
         <x:v>1136</x:v>
@@ -6526,7 +6521,7 @@
     </x:row>
     <x:row r="266" spans="1:11" outlineLevel="3">
       <x:c r="B266" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C266" s="41" t="n">
         <x:v>1021</x:v>
@@ -6550,7 +6545,7 @@
     </x:row>
     <x:row r="267" spans="1:11" outlineLevel="3">
       <x:c r="B267" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C267" s="41" t="n">
         <x:v>1032</x:v>
@@ -6574,7 +6569,7 @@
     </x:row>
     <x:row r="268" spans="1:11" outlineLevel="3">
       <x:c r="B268" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C268" s="41" t="n">
         <x:v>1122</x:v>
@@ -6598,7 +6593,7 @@
     </x:row>
     <x:row r="269" spans="1:11" outlineLevel="3">
       <x:c r="B269" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C269" s="41" t="n">
         <x:v>1121</x:v>
@@ -6622,7 +6617,7 @@
     </x:row>
     <x:row r="270" spans="1:11" outlineLevel="3">
       <x:c r="B270" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C270" s="41" t="n">
         <x:v>1022</x:v>
@@ -6646,7 +6641,7 @@
     </x:row>
     <x:row r="271" spans="1:11" outlineLevel="1">
       <x:c r="B271" s="34" t="s">
-        <x:v>106</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C271" s="34" t="s"/>
       <x:c r="D271" s="35" t="s"/>
@@ -6662,7 +6657,7 @@
       <x:c r="B272" s="34" t="s"/>
       <x:c r="C272" s="34" t="s"/>
       <x:c r="D272" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E272" s="36" t="s"/>
       <x:c r="F272" s="37" t="s"/>
@@ -6674,13 +6669,13 @@
     </x:row>
     <x:row r="273" spans="1:11" outlineLevel="3">
       <x:c r="B273" s="40" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C273" s="41" t="n">
         <x:v>1101</x:v>
       </x:c>
       <x:c r="D273" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E273" s="42">
         <x:v>32693</x:v>
@@ -6700,7 +6695,7 @@
     </x:row>
     <x:row r="274" spans="1:11" outlineLevel="3">
       <x:c r="B274" s="40" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C274" s="41" t="n">
         <x:v>1051</x:v>
@@ -6724,7 +6719,7 @@
     </x:row>
     <x:row r="275" spans="1:11" outlineLevel="1">
       <x:c r="B275" s="34" t="s">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C275" s="34" t="s"/>
       <x:c r="D275" s="35" t="s"/>
@@ -6740,7 +6735,7 @@
       <x:c r="B276" s="34" t="s"/>
       <x:c r="C276" s="34" t="s"/>
       <x:c r="D276" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E276" s="36" t="s"/>
       <x:c r="F276" s="37" t="s"/>
@@ -6752,13 +6747,13 @@
     </x:row>
     <x:row r="277" spans="1:11" outlineLevel="3">
       <x:c r="B277" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C277" s="41" t="n">
         <x:v>1052</x:v>
       </x:c>
       <x:c r="D277" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E277" s="42">
         <x:v>32515</x:v>
@@ -6778,7 +6773,7 @@
     </x:row>
     <x:row r="278" spans="1:11" outlineLevel="3">
       <x:c r="B278" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C278" s="41" t="n">
         <x:v>1155</x:v>
@@ -6802,7 +6797,7 @@
     </x:row>
     <x:row r="279" spans="1:11" outlineLevel="3">
       <x:c r="B279" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C279" s="41" t="n">
         <x:v>1152</x:v>
@@ -6826,7 +6821,7 @@
     </x:row>
     <x:row r="280" spans="1:11" outlineLevel="3">
       <x:c r="B280" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C280" s="41" t="n">
         <x:v>1163</x:v>
@@ -6850,7 +6845,7 @@
     </x:row>
     <x:row r="281" spans="1:11" outlineLevel="3">
       <x:c r="B281" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C281" s="41" t="n">
         <x:v>1087</x:v>
@@ -6874,7 +6869,7 @@
     </x:row>
     <x:row r="282" spans="1:11" outlineLevel="3">
       <x:c r="B282" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C282" s="41" t="n">
         <x:v>1055</x:v>
@@ -6898,7 +6893,7 @@
     </x:row>
     <x:row r="283" spans="1:11" outlineLevel="3">
       <x:c r="B283" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C283" s="41" t="n">
         <x:v>1003</x:v>
@@ -6922,7 +6917,7 @@
     </x:row>
     <x:row r="284" spans="1:11" outlineLevel="3">
       <x:c r="B284" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C284" s="41" t="n">
         <x:v>1255</x:v>
@@ -6948,7 +6943,7 @@
       <x:c r="B285" s="34" t="s"/>
       <x:c r="C285" s="34" t="s"/>
       <x:c r="D285" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E285" s="36" t="s"/>
       <x:c r="F285" s="37" t="s"/>
@@ -6960,13 +6955,13 @@
     </x:row>
     <x:row r="286" spans="1:11" outlineLevel="3">
       <x:c r="B286" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C286" s="41" t="n">
         <x:v>1275</x:v>
       </x:c>
       <x:c r="D286" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E286" s="42">
         <x:v>34690</x:v>
@@ -6986,7 +6981,7 @@
     </x:row>
     <x:row r="287" spans="1:11" outlineLevel="3">
       <x:c r="B287" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C287" s="41" t="n">
         <x:v>1075</x:v>
@@ -7012,7 +7007,7 @@
       <x:c r="B288" s="34" t="s"/>
       <x:c r="C288" s="34" t="s"/>
       <x:c r="D288" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E288" s="36" t="s"/>
       <x:c r="F288" s="37" t="s"/>
@@ -7024,13 +7019,13 @@
     </x:row>
     <x:row r="289" spans="1:11" outlineLevel="3">
       <x:c r="B289" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C289" s="41" t="n">
         <x:v>1067</x:v>
       </x:c>
       <x:c r="D289" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E289" s="42">
         <x:v>32600</x:v>
@@ -7050,7 +7045,7 @@
     </x:row>
     <x:row r="290" spans="1:11" outlineLevel="1">
       <x:c r="B290" s="34" t="s">
-        <x:v>110</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C290" s="34" t="s"/>
       <x:c r="D290" s="35" t="s"/>
@@ -7066,7 +7061,7 @@
       <x:c r="B291" s="34" t="s"/>
       <x:c r="C291" s="34" t="s"/>
       <x:c r="D291" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E291" s="36" t="s"/>
       <x:c r="F291" s="37" t="s"/>
@@ -7078,13 +7073,13 @@
     </x:row>
     <x:row r="292" spans="1:11" outlineLevel="3">
       <x:c r="B292" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C292" s="41" t="n">
         <x:v>1171</x:v>
       </x:c>
       <x:c r="D292" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E292" s="42">
         <x:v>34525</x:v>
@@ -7104,7 +7099,7 @@
     </x:row>
     <x:row r="293" spans="1:11" outlineLevel="3">
       <x:c r="B293" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C293" s="41" t="n">
         <x:v>1271</x:v>
@@ -7128,7 +7123,7 @@
     </x:row>
     <x:row r="294" spans="1:11" outlineLevel="3">
       <x:c r="B294" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C294" s="41" t="n">
         <x:v>1071</x:v>
@@ -7154,7 +7149,7 @@
       <x:c r="B295" s="34" t="s"/>
       <x:c r="C295" s="34" t="s"/>
       <x:c r="D295" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E295" s="36" t="s"/>
       <x:c r="F295" s="37" t="s"/>
@@ -7166,13 +7161,13 @@
     </x:row>
     <x:row r="296" spans="1:11" outlineLevel="3">
       <x:c r="B296" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C296" s="41" t="n">
         <x:v>1011</x:v>
       </x:c>
       <x:c r="D296" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E296" s="42">
         <x:v>32282</x:v>
@@ -7192,7 +7187,7 @@
     </x:row>
     <x:row r="297" spans="1:11" outlineLevel="3">
       <x:c r="B297" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C297" s="41" t="n">
         <x:v>1111</x:v>
@@ -7218,7 +7213,7 @@
       <x:c r="B298" s="34" t="s"/>
       <x:c r="C298" s="34" t="s"/>
       <x:c r="D298" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E298" s="36" t="s"/>
       <x:c r="F298" s="37" t="s"/>
@@ -7230,13 +7225,13 @@
     </x:row>
     <x:row r="299" spans="1:11" outlineLevel="3">
       <x:c r="B299" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C299" s="41" t="n">
         <x:v>1035</x:v>
       </x:c>
       <x:c r="D299" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E299" s="42">
         <x:v>32372</x:v>
@@ -7258,7 +7253,7 @@
       <x:c r="B300" s="34" t="s"/>
       <x:c r="C300" s="34" t="s"/>
       <x:c r="D300" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E300" s="36" t="s"/>
       <x:c r="F300" s="37" t="s"/>
@@ -7270,13 +7265,13 @@
     </x:row>
     <x:row r="301" spans="1:11" outlineLevel="3">
       <x:c r="B301" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C301" s="41" t="n">
         <x:v>1154</x:v>
       </x:c>
       <x:c r="D301" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E301" s="42">
         <x:v>34455</x:v>
@@ -7296,7 +7291,7 @@
     </x:row>
     <x:row r="302" spans="1:11" outlineLevel="1">
       <x:c r="B302" s="34" t="s">
-        <x:v>112</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C302" s="34" t="s"/>
       <x:c r="D302" s="35" t="s"/>
@@ -7312,7 +7307,7 @@
       <x:c r="B303" s="34" t="s"/>
       <x:c r="C303" s="34" t="s"/>
       <x:c r="D303" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E303" s="36" t="s"/>
       <x:c r="F303" s="37" t="s"/>
@@ -7324,13 +7319,13 @@
     </x:row>
     <x:row r="304" spans="1:11" outlineLevel="3">
       <x:c r="B304" s="40" t="s">
-        <x:v>113</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C304" s="41" t="n">
         <x:v>1053</x:v>
       </x:c>
       <x:c r="D304" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E304" s="42">
         <x:v>32524</x:v>
@@ -7350,7 +7345,7 @@
     </x:row>
     <x:row r="305" spans="1:11" outlineLevel="1">
       <x:c r="B305" s="34" t="s">
-        <x:v>114</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C305" s="34" t="s"/>
       <x:c r="D305" s="35" t="s"/>
@@ -7366,7 +7361,7 @@
       <x:c r="B306" s="34" t="s"/>
       <x:c r="C306" s="34" t="s"/>
       <x:c r="D306" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E306" s="36" t="s"/>
       <x:c r="F306" s="37" t="s"/>
@@ -7378,13 +7373,13 @@
     </x:row>
     <x:row r="307" spans="1:11" outlineLevel="3">
       <x:c r="B307" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C307" s="41" t="n">
         <x:v>1059</x:v>
       </x:c>
       <x:c r="D307" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E307" s="42">
         <x:v>32564</x:v>
@@ -7404,7 +7399,7 @@
     </x:row>
     <x:row r="308" spans="1:11" outlineLevel="3">
       <x:c r="B308" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C308" s="41" t="n">
         <x:v>1072</x:v>
@@ -7430,7 +7425,7 @@
       <x:c r="B309" s="34" t="s"/>
       <x:c r="C309" s="34" t="s"/>
       <x:c r="D309" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E309" s="36" t="s"/>
       <x:c r="F309" s="37" t="s"/>
@@ -7442,13 +7437,13 @@
     </x:row>
     <x:row r="310" spans="1:11" outlineLevel="3">
       <x:c r="B310" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C310" s="41" t="n">
         <x:v>1280</x:v>
       </x:c>
       <x:c r="D310" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E310" s="42">
         <x:v>34694</x:v>
@@ -7468,7 +7463,7 @@
     </x:row>
     <x:row r="311" spans="1:11" outlineLevel="3">
       <x:c r="B311" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C311" s="41" t="n">
         <x:v>1080</x:v>
@@ -7492,7 +7487,7 @@
     </x:row>
     <x:row r="312" spans="1:11" outlineLevel="3">
       <x:c r="B312" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C312" s="41" t="n">
         <x:v>1180</x:v>
@@ -7518,7 +7513,7 @@
       <x:c r="B313" s="34" t="s"/>
       <x:c r="C313" s="34" t="s"/>
       <x:c r="D313" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E313" s="36" t="s"/>
       <x:c r="F313" s="37" t="s"/>
@@ -7530,13 +7525,13 @@
     </x:row>
     <x:row r="314" spans="1:11" outlineLevel="3">
       <x:c r="B314" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C314" s="41" t="n">
         <x:v>1105</x:v>
       </x:c>
       <x:c r="D314" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E314" s="42">
         <x:v>33806</x:v>
@@ -7556,7 +7551,7 @@
     </x:row>
     <x:row r="315" spans="1:11" outlineLevel="3">
       <x:c r="B315" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C315" s="41" t="n">
         <x:v>1005</x:v>
@@ -7580,7 +7575,7 @@
     </x:row>
     <x:row r="316" spans="1:11" outlineLevel="3">
       <x:c r="B316" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C316" s="41" t="n">
         <x:v>1305</x:v>
@@ -7604,7 +7599,7 @@
     </x:row>
     <x:row r="317" spans="1:11" outlineLevel="3">
       <x:c r="B317" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C317" s="41" t="n">
         <x:v>1266</x:v>
@@ -7628,7 +7623,7 @@
     </x:row>
     <x:row r="318" spans="1:11" outlineLevel="1">
       <x:c r="B318" s="34" t="s">
-        <x:v>116</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C318" s="34" t="s"/>
       <x:c r="D318" s="35" t="s"/>
@@ -7644,7 +7639,7 @@
       <x:c r="B319" s="34" t="s"/>
       <x:c r="C319" s="34" t="s"/>
       <x:c r="D319" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E319" s="36" t="s"/>
       <x:c r="F319" s="37" t="s"/>
@@ -7656,13 +7651,13 @@
     </x:row>
     <x:row r="320" spans="1:11" outlineLevel="3">
       <x:c r="B320" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C320" s="41" t="n">
         <x:v>1119</x:v>
       </x:c>
       <x:c r="D320" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E320" s="42">
         <x:v>34104</x:v>
@@ -7682,7 +7677,7 @@
     </x:row>
     <x:row r="321" spans="1:11" outlineLevel="3">
       <x:c r="B321" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C321" s="41" t="n">
         <x:v>1036</x:v>
@@ -7708,7 +7703,7 @@
       <x:c r="B322" s="34" t="s"/>
       <x:c r="C322" s="34" t="s"/>
       <x:c r="D322" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E322" s="36" t="s"/>
       <x:c r="F322" s="37" t="s"/>
@@ -7720,13 +7715,13 @@
     </x:row>
     <x:row r="323" spans="1:11" outlineLevel="3">
       <x:c r="B323" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C323" s="41" t="n">
         <x:v>1195</x:v>
       </x:c>
       <x:c r="D323" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E323" s="42">
         <x:v>34583</x:v>
@@ -7746,7 +7741,7 @@
     </x:row>
     <x:row r="324" spans="1:11" outlineLevel="1">
       <x:c r="B324" s="34" t="s">
-        <x:v>118</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C324" s="34" t="s"/>
       <x:c r="D324" s="35" t="s"/>
@@ -7762,7 +7757,7 @@
       <x:c r="B325" s="34" t="s"/>
       <x:c r="C325" s="34" t="s"/>
       <x:c r="D325" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E325" s="36" t="s"/>
       <x:c r="F325" s="37" t="s"/>
@@ -7774,13 +7769,13 @@
     </x:row>
     <x:row r="326" spans="1:11" outlineLevel="3">
       <x:c r="B326" s="40" t="s">
-        <x:v>119</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C326" s="41" t="n">
         <x:v>1115</x:v>
       </x:c>
       <x:c r="D326" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E326" s="42">
         <x:v>34041</x:v>
@@ -7800,7 +7795,7 @@
     </x:row>
     <x:row r="327" spans="1:11" outlineLevel="1">
       <x:c r="B327" s="34" t="s">
-        <x:v>120</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C327" s="34" t="s"/>
       <x:c r="D327" s="35" t="s"/>
@@ -7816,7 +7811,7 @@
       <x:c r="B328" s="34" t="s"/>
       <x:c r="C328" s="34" t="s"/>
       <x:c r="D328" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E328" s="36" t="s"/>
       <x:c r="F328" s="37" t="s"/>
@@ -7828,13 +7823,13 @@
     </x:row>
     <x:row r="329" spans="1:11" outlineLevel="3">
       <x:c r="B329" s="40" t="s">
-        <x:v>121</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C329" s="41" t="n">
         <x:v>1070</x:v>
       </x:c>
       <x:c r="D329" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E329" s="42">
         <x:v>32606</x:v>
@@ -7854,7 +7849,7 @@
     </x:row>
     <x:row r="330" spans="1:11" outlineLevel="1">
       <x:c r="B330" s="34" t="s">
-        <x:v>122</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C330" s="34" t="s"/>
       <x:c r="D330" s="35" t="s"/>
@@ -7870,7 +7865,7 @@
       <x:c r="B331" s="34" t="s"/>
       <x:c r="C331" s="34" t="s"/>
       <x:c r="D331" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E331" s="36" t="s"/>
       <x:c r="F331" s="37" t="s"/>
@@ -7882,13 +7877,13 @@
     </x:row>
     <x:row r="332" spans="1:11" outlineLevel="3">
       <x:c r="B332" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C332" s="41" t="n">
         <x:v>1250</x:v>
       </x:c>
       <x:c r="D332" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E332" s="42">
         <x:v>34662</x:v>
@@ -7908,7 +7903,7 @@
     </x:row>
     <x:row r="333" spans="1:11" outlineLevel="3">
       <x:c r="B333" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C333" s="41" t="n">
         <x:v>1350</x:v>
@@ -7932,7 +7927,7 @@
     </x:row>
     <x:row r="334" spans="1:11" outlineLevel="3">
       <x:c r="B334" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C334" s="41" t="n">
         <x:v>1050</x:v>
@@ -7956,7 +7951,7 @@
     </x:row>
     <x:row r="335" spans="1:11" outlineLevel="3">
       <x:c r="B335" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C335" s="41" t="n">
         <x:v>1150</x:v>
@@ -7980,7 +7975,7 @@
     </x:row>
     <x:row r="336" spans="1:11" outlineLevel="1">
       <x:c r="B336" s="34" t="s">
-        <x:v>124</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C336" s="34" t="s"/>
       <x:c r="D336" s="35" t="s"/>
@@ -7996,7 +7991,7 @@
       <x:c r="B337" s="34" t="s"/>
       <x:c r="C337" s="34" t="s"/>
       <x:c r="D337" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E337" s="36" t="s"/>
       <x:c r="F337" s="37" t="s"/>
@@ -8008,13 +8003,13 @@
     </x:row>
     <x:row r="338" spans="1:11" outlineLevel="3">
       <x:c r="B338" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C338" s="41" t="n">
         <x:v>1060</x:v>
       </x:c>
       <x:c r="D338" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E338" s="42">
         <x:v>32568</x:v>
@@ -8034,7 +8029,7 @@
     </x:row>
     <x:row r="339" spans="1:11" outlineLevel="3">
       <x:c r="B339" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C339" s="41" t="n">
         <x:v>1160</x:v>
@@ -8060,7 +8055,7 @@
       <x:c r="B340" s="34" t="s"/>
       <x:c r="C340" s="34" t="s"/>
       <x:c r="D340" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E340" s="36" t="s"/>
       <x:c r="F340" s="37" t="s"/>
@@ -8072,13 +8067,13 @@
     </x:row>
     <x:row r="341" spans="1:11" outlineLevel="3">
       <x:c r="B341" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C341" s="41" t="n">
         <x:v>1202</x:v>
       </x:c>
       <x:c r="D341" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E341" s="42">
         <x:v>34613</x:v>
@@ -8098,7 +8093,7 @@
     </x:row>
     <x:row r="342" spans="1:11" outlineLevel="3">
       <x:c r="B342" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C342" s="41" t="n">
         <x:v>1178</x:v>
@@ -8122,7 +8117,7 @@
     </x:row>
     <x:row r="343" spans="1:11" outlineLevel="3">
       <x:c r="B343" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C343" s="41" t="n">
         <x:v>1302</x:v>
@@ -8146,7 +8141,7 @@
     </x:row>
     <x:row r="344" spans="1:11" outlineLevel="3">
       <x:c r="B344" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C344" s="41" t="n">
         <x:v>1278</x:v>
@@ -8170,7 +8165,7 @@
     </x:row>
     <x:row r="345" spans="1:11" outlineLevel="3">
       <x:c r="B345" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C345" s="41" t="n">
         <x:v>1102</x:v>
@@ -8196,7 +8191,7 @@
       <x:c r="B346" s="34" t="s"/>
       <x:c r="C346" s="34" t="s"/>
       <x:c r="D346" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E346" s="36" t="s"/>
       <x:c r="F346" s="37" t="s"/>
@@ -8208,13 +8203,13 @@
     </x:row>
     <x:row r="347" spans="1:11" outlineLevel="3">
       <x:c r="B347" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C347" s="41" t="n">
         <x:v>1073</x:v>
       </x:c>
       <x:c r="D347" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E347" s="42">
         <x:v>32614</x:v>
@@ -8234,7 +8229,7 @@
     </x:row>
     <x:row r="348" spans="1:11" outlineLevel="3">
       <x:c r="B348" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C348" s="41" t="n">
         <x:v>1173</x:v>
@@ -8258,7 +8253,7 @@
     </x:row>
     <x:row r="349" spans="1:11" outlineLevel="1">
       <x:c r="B349" s="34" t="s">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C349" s="34" t="s"/>
       <x:c r="D349" s="35" t="s"/>
@@ -8274,7 +8269,7 @@
       <x:c r="B350" s="34" t="s"/>
       <x:c r="C350" s="34" t="s"/>
       <x:c r="D350" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E350" s="36" t="s"/>
       <x:c r="F350" s="37" t="s"/>
@@ -8286,13 +8281,13 @@
     </x:row>
     <x:row r="351" spans="1:11" outlineLevel="3">
       <x:c r="B351" s="40" t="s">
-        <x:v>127</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C351" s="41" t="n">
         <x:v>1296</x:v>
       </x:c>
       <x:c r="D351" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E351" s="42">
         <x:v>34707</x:v>
@@ -8312,7 +8307,7 @@
     </x:row>
     <x:row r="352" spans="1:11" outlineLevel="1">
       <x:c r="B352" s="34" t="s">
-        <x:v>128</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C352" s="34" t="s"/>
       <x:c r="D352" s="35" t="s"/>
@@ -8328,7 +8323,7 @@
       <x:c r="B353" s="34" t="s"/>
       <x:c r="C353" s="34" t="s"/>
       <x:c r="D353" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E353" s="36" t="s"/>
       <x:c r="F353" s="37" t="s"/>
@@ -8340,13 +8335,13 @@
     </x:row>
     <x:row r="354" spans="1:11" outlineLevel="3">
       <x:c r="B354" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C354" s="41" t="n">
         <x:v>1033</x:v>
       </x:c>
       <x:c r="D354" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E354" s="42">
         <x:v>32357</x:v>
@@ -8368,7 +8363,7 @@
       <x:c r="B355" s="34" t="s"/>
       <x:c r="C355" s="34" t="s"/>
       <x:c r="D355" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E355" s="36" t="s"/>
       <x:c r="F355" s="37" t="s"/>
@@ -8380,13 +8375,13 @@
     </x:row>
     <x:row r="356" spans="1:11" outlineLevel="3">
       <x:c r="B356" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C356" s="41" t="n">
         <x:v>1124</x:v>
       </x:c>
       <x:c r="D356" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E356" s="42">
         <x:v>34213</x:v>
@@ -8408,7 +8403,7 @@
       <x:c r="B357" s="34" t="s"/>
       <x:c r="C357" s="34" t="s"/>
       <x:c r="D357" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E357" s="36" t="s"/>
       <x:c r="F357" s="37" t="s"/>
@@ -8420,13 +8415,13 @@
     </x:row>
     <x:row r="358" spans="1:11" outlineLevel="3">
       <x:c r="B358" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C358" s="41" t="n">
         <x:v>1200</x:v>
       </x:c>
       <x:c r="D358" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E358" s="42">
         <x:v>34597</x:v>
@@ -8446,7 +8441,7 @@
     </x:row>
     <x:row r="359" spans="1:11" outlineLevel="3">
       <x:c r="B359" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C359" s="41" t="n">
         <x:v>1300</x:v>
@@ -8470,7 +8465,7 @@
     </x:row>
     <x:row r="360" spans="1:11" outlineLevel="3">
       <x:c r="B360" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C360" s="41" t="n">
         <x:v>1100</x:v>
@@ -8496,7 +8491,7 @@
       <x:c r="B361" s="34" t="s"/>
       <x:c r="C361" s="34" t="s"/>
       <x:c r="D361" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E361" s="36" t="s"/>
       <x:c r="F361" s="37" t="s"/>
@@ -8508,13 +8503,13 @@
     </x:row>
     <x:row r="362" spans="1:11" outlineLevel="3">
       <x:c r="B362" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C362" s="41" t="n">
         <x:v>1127</x:v>
       </x:c>
       <x:c r="D362" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E362" s="42">
         <x:v>34244</x:v>
@@ -8534,7 +8529,7 @@
     </x:row>
     <x:row r="363" spans="1:11" outlineLevel="3">
       <x:c r="B363" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C363" s="41" t="n">
         <x:v>1207</x:v>
@@ -8558,7 +8553,7 @@
     </x:row>
     <x:row r="364" spans="1:11" outlineLevel="3">
       <x:c r="B364" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C364" s="41" t="n">
         <x:v>1027</x:v>
@@ -8582,7 +8577,7 @@
     </x:row>
     <x:row r="365" spans="1:11" outlineLevel="3">
       <x:c r="B365" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C365" s="41" t="n">
         <x:v>1107</x:v>
@@ -8606,7 +8601,7 @@
     </x:row>
     <x:row r="366" spans="1:11" outlineLevel="3">
       <x:c r="B366" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C366" s="41" t="n">
         <x:v>1007</x:v>
@@ -8630,7 +8625,7 @@
     </x:row>
     <x:row r="367" spans="1:11" outlineLevel="1">
       <x:c r="B367" s="34" t="s">
-        <x:v>130</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C367" s="34" t="s"/>
       <x:c r="D367" s="35" t="s"/>
@@ -8646,7 +8641,7 @@
       <x:c r="B368" s="34" t="s"/>
       <x:c r="C368" s="34" t="s"/>
       <x:c r="D368" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E368" s="36" t="s"/>
       <x:c r="F368" s="37" t="s"/>
@@ -8658,13 +8653,13 @@
     </x:row>
     <x:row r="369" spans="1:11" outlineLevel="3">
       <x:c r="B369" s="40" t="s">
-        <x:v>131</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C369" s="41" t="n">
         <x:v>1140</x:v>
       </x:c>
       <x:c r="D369" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E369" s="42">
         <x:v>34315</x:v>
@@ -8684,7 +8679,7 @@
     </x:row>
     <x:row r="370" spans="1:11" outlineLevel="3">
       <x:c r="B370" s="40" t="s">
-        <x:v>131</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C370" s="41" t="n">
         <x:v>1040</x:v>

</xml_diff>

<commit_message>
Add multiple levels totallabel support (#205)
* Add summary tag with label in group feature

* Add summary tag with label in group feature

* Add multiple levels totallabel feature

* Reformat
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
+++ b/tests/Gauges/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <x:si>
     <x:t>Formulas in group row</x:t>
   </x:si>
@@ -48,9 +48,6 @@
   <x:si>
     <x:t>Amount
 paid</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Action Club </x:t>
@@ -1323,9 +1320,7 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <x:c r="B5" s="34" t="s">
-        <x:v>9</x:v>
-      </x:c>
+      <x:c r="B5" s="34" t="s"/>
       <x:c r="C5" s="34" t="s"/>
       <x:c r="D5" s="35" t="s"/>
       <x:c r="E5" s="36" t="s"/>
@@ -1338,7 +1333,7 @@
     </x:row>
     <x:row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <x:c r="B6" s="34" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C6" s="34" t="s"/>
       <x:c r="D6" s="35" t="s"/>
@@ -1354,7 +1349,7 @@
       <x:c r="B7" s="34" t="s"/>
       <x:c r="C7" s="34" t="s"/>
       <x:c r="D7" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E7" s="36" t="s"/>
       <x:c r="F7" s="37" t="s"/>
@@ -1366,13 +1361,13 @@
     </x:row>
     <x:row r="8" spans="1:11" outlineLevel="3">
       <x:c r="B8" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C8" s="41" t="n">
         <x:v>1014</x:v>
       </x:c>
       <x:c r="D8" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E8" s="42">
         <x:v>32289</x:v>
@@ -1394,7 +1389,7 @@
       <x:c r="B9" s="34" t="s"/>
       <x:c r="C9" s="34" t="s"/>
       <x:c r="D9" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E9" s="36" t="s"/>
       <x:c r="F9" s="37" t="s"/>
@@ -1406,13 +1401,13 @@
     </x:row>
     <x:row r="10" spans="1:11" outlineLevel="3">
       <x:c r="B10" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C10" s="41" t="n">
         <x:v>1129</x:v>
       </x:c>
       <x:c r="D10" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E10" s="42">
         <x:v>34261</x:v>
@@ -1432,7 +1427,7 @@
     </x:row>
     <x:row r="11" spans="1:11" outlineLevel="3">
       <x:c r="B11" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C11" s="41" t="n">
         <x:v>1029</x:v>
@@ -1458,7 +1453,7 @@
       <x:c r="B12" s="34" t="s"/>
       <x:c r="C12" s="34" t="s"/>
       <x:c r="D12" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E12" s="36" t="s"/>
       <x:c r="F12" s="37" t="s"/>
@@ -1470,13 +1465,13 @@
     </x:row>
     <x:row r="13" spans="1:11" outlineLevel="3">
       <x:c r="B13" s="40" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C13" s="41" t="n">
         <x:v>1038</x:v>
       </x:c>
       <x:c r="D13" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E13" s="42">
         <x:v>32382</x:v>
@@ -1496,7 +1491,7 @@
     </x:row>
     <x:row r="14" spans="1:11" outlineLevel="1">
       <x:c r="B14" s="34" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C14" s="34" t="s"/>
       <x:c r="D14" s="35" t="s"/>
@@ -1512,7 +1507,7 @@
       <x:c r="B15" s="34" t="s"/>
       <x:c r="C15" s="34" t="s"/>
       <x:c r="D15" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E15" s="36" t="s"/>
       <x:c r="F15" s="37" t="s"/>
@@ -1524,13 +1519,13 @@
     </x:row>
     <x:row r="16" spans="1:11" outlineLevel="3">
       <x:c r="B16" s="40" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C16" s="41" t="n">
         <x:v>1039</x:v>
       </x:c>
       <x:c r="D16" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E16" s="42">
         <x:v>32387</x:v>
@@ -1550,7 +1545,7 @@
     </x:row>
     <x:row r="17" spans="1:11" outlineLevel="1">
       <x:c r="B17" s="34" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C17" s="34" t="s"/>
       <x:c r="D17" s="35" t="s"/>
@@ -1566,7 +1561,7 @@
       <x:c r="B18" s="34" t="s"/>
       <x:c r="C18" s="34" t="s"/>
       <x:c r="D18" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E18" s="36" t="s"/>
       <x:c r="F18" s="37" t="s"/>
@@ -1578,13 +1573,13 @@
     </x:row>
     <x:row r="19" spans="1:11" outlineLevel="3">
       <x:c r="B19" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C19" s="41" t="n">
         <x:v>1017</x:v>
       </x:c>
       <x:c r="D19" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E19" s="42">
         <x:v>32307</x:v>
@@ -1604,7 +1599,7 @@
     </x:row>
     <x:row r="20" spans="1:11" outlineLevel="3">
       <x:c r="B20" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C20" s="41" t="n">
         <x:v>1217</x:v>
@@ -1628,7 +1623,7 @@
     </x:row>
     <x:row r="21" spans="1:11" outlineLevel="3">
       <x:c r="B21" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C21" s="41" t="n">
         <x:v>1117</x:v>
@@ -1652,7 +1647,7 @@
     </x:row>
     <x:row r="22" spans="1:11" outlineLevel="3">
       <x:c r="B22" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C22" s="41" t="n">
         <x:v>1317</x:v>
@@ -1678,7 +1673,7 @@
       <x:c r="B23" s="34" t="s"/>
       <x:c r="C23" s="34" t="s"/>
       <x:c r="D23" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E23" s="36" t="s"/>
       <x:c r="F23" s="37" t="s"/>
@@ -1690,13 +1685,13 @@
     </x:row>
     <x:row r="24" spans="1:11" outlineLevel="3">
       <x:c r="B24" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C24" s="41" t="n">
         <x:v>1137</x:v>
       </x:c>
       <x:c r="D24" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E24" s="42">
         <x:v>34300</x:v>
@@ -1716,7 +1711,7 @@
     </x:row>
     <x:row r="25" spans="1:11" outlineLevel="3">
       <x:c r="B25" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C25" s="41" t="n">
         <x:v>1037</x:v>
@@ -1740,7 +1735,7 @@
     </x:row>
     <x:row r="26" spans="1:11" outlineLevel="3">
       <x:c r="B26" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C26" s="41" t="n">
         <x:v>1099</x:v>
@@ -1766,7 +1761,7 @@
       <x:c r="B27" s="34" t="s"/>
       <x:c r="C27" s="34" t="s"/>
       <x:c r="D27" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="36" t="s"/>
       <x:c r="F27" s="37" t="s"/>
@@ -1778,13 +1773,13 @@
     </x:row>
     <x:row r="28" spans="1:11" outlineLevel="3">
       <x:c r="B28" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C28" s="41" t="n">
         <x:v>1294</x:v>
       </x:c>
       <x:c r="D28" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E28" s="42">
         <x:v>34703</x:v>
@@ -1804,7 +1799,7 @@
     </x:row>
     <x:row r="29" spans="1:11" outlineLevel="3">
       <x:c r="B29" s="40" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C29" s="41" t="n">
         <x:v>1074</x:v>
@@ -1828,7 +1823,7 @@
     </x:row>
     <x:row r="30" spans="1:11" outlineLevel="1">
       <x:c r="B30" s="34" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C30" s="34" t="s"/>
       <x:c r="D30" s="35" t="s"/>
@@ -1844,7 +1839,7 @@
       <x:c r="B31" s="34" t="s"/>
       <x:c r="C31" s="34" t="s"/>
       <x:c r="D31" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E31" s="36" t="s"/>
       <x:c r="F31" s="37" t="s"/>
@@ -1856,13 +1851,13 @@
     </x:row>
     <x:row r="32" spans="1:11" outlineLevel="3">
       <x:c r="B32" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C32" s="41" t="n">
         <x:v>1204</x:v>
       </x:c>
       <x:c r="D32" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E32" s="42">
         <x:v>34625</x:v>
@@ -1884,7 +1879,7 @@
       <x:c r="B33" s="34" t="s"/>
       <x:c r="C33" s="34" t="s"/>
       <x:c r="D33" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E33" s="36" t="s"/>
       <x:c r="F33" s="37" t="s"/>
@@ -1896,13 +1891,13 @@
     </x:row>
     <x:row r="34" spans="1:11" outlineLevel="3">
       <x:c r="B34" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C34" s="41" t="n">
         <x:v>1355</x:v>
       </x:c>
       <x:c r="D34" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E34" s="42">
         <x:v>34735</x:v>
@@ -1922,7 +1917,7 @@
     </x:row>
     <x:row r="35" spans="1:11" outlineLevel="3">
       <x:c r="B35" s="40" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C35" s="41" t="n">
         <x:v>1263</x:v>
@@ -1946,7 +1941,7 @@
     </x:row>
     <x:row r="36" spans="1:11" outlineLevel="1">
       <x:c r="B36" s="34" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C36" s="34" t="s"/>
       <x:c r="D36" s="35" t="s"/>
@@ -1962,7 +1957,7 @@
       <x:c r="B37" s="34" t="s"/>
       <x:c r="C37" s="34" t="s"/>
       <x:c r="D37" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E37" s="36" t="s"/>
       <x:c r="F37" s="37" t="s"/>
@@ -1974,13 +1969,13 @@
     </x:row>
     <x:row r="38" spans="1:11" outlineLevel="3">
       <x:c r="B38" s="40" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C38" s="41" t="n">
         <x:v>1065</x:v>
       </x:c>
       <x:c r="D38" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E38" s="42">
         <x:v>32593</x:v>
@@ -2000,7 +1995,7 @@
     </x:row>
     <x:row r="39" spans="1:11" outlineLevel="1">
       <x:c r="B39" s="34" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C39" s="34" t="s"/>
       <x:c r="D39" s="35" t="s"/>
@@ -2016,7 +2011,7 @@
       <x:c r="B40" s="34" t="s"/>
       <x:c r="C40" s="34" t="s"/>
       <x:c r="D40" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E40" s="36" t="s"/>
       <x:c r="F40" s="37" t="s"/>
@@ -2028,13 +2023,13 @@
     </x:row>
     <x:row r="41" spans="1:11" outlineLevel="3">
       <x:c r="B41" s="40" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C41" s="41" t="n">
         <x:v>1042</x:v>
       </x:c>
       <x:c r="D41" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E41" s="42">
         <x:v>32411</x:v>
@@ -2054,7 +2049,7 @@
     </x:row>
     <x:row r="42" spans="1:11" outlineLevel="3">
       <x:c r="B42" s="40" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C42" s="41" t="n">
         <x:v>1142</x:v>
@@ -2078,7 +2073,7 @@
     </x:row>
     <x:row r="43" spans="1:11" outlineLevel="1">
       <x:c r="B43" s="34" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C43" s="34" t="s"/>
       <x:c r="D43" s="35" t="s"/>
@@ -2094,7 +2089,7 @@
       <x:c r="B44" s="34" t="s"/>
       <x:c r="C44" s="34" t="s"/>
       <x:c r="D44" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E44" s="36" t="s"/>
       <x:c r="F44" s="37" t="s"/>
@@ -2106,13 +2101,13 @@
     </x:row>
     <x:row r="45" spans="1:11" outlineLevel="3">
       <x:c r="B45" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C45" s="41" t="n">
         <x:v>1079</x:v>
       </x:c>
       <x:c r="D45" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E45" s="42">
         <x:v>32632</x:v>
@@ -2132,7 +2127,7 @@
     </x:row>
     <x:row r="46" spans="1:11" outlineLevel="3">
       <x:c r="B46" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C46" s="41" t="n">
         <x:v>1153</x:v>
@@ -2156,7 +2151,7 @@
     </x:row>
     <x:row r="47" spans="1:11" outlineLevel="3">
       <x:c r="B47" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C47" s="41" t="n">
         <x:v>1253</x:v>
@@ -2182,7 +2177,7 @@
       <x:c r="B48" s="34" t="s"/>
       <x:c r="C48" s="34" t="s"/>
       <x:c r="D48" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E48" s="36" t="s"/>
       <x:c r="F48" s="37" t="s"/>
@@ -2194,13 +2189,13 @@
     </x:row>
     <x:row r="49" spans="1:11" outlineLevel="3">
       <x:c r="B49" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C49" s="41" t="n">
         <x:v>1106</x:v>
       </x:c>
       <x:c r="D49" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E49" s="42">
         <x:v>33870</x:v>
@@ -2220,7 +2215,7 @@
     </x:row>
     <x:row r="50" spans="1:11" outlineLevel="3">
       <x:c r="B50" s="40" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C50" s="41" t="n">
         <x:v>1006</x:v>
@@ -2244,7 +2239,7 @@
     </x:row>
     <x:row r="51" spans="1:11" outlineLevel="1">
       <x:c r="B51" s="34" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C51" s="34" t="s"/>
       <x:c r="D51" s="35" t="s"/>
@@ -2260,7 +2255,7 @@
       <x:c r="B52" s="34" t="s"/>
       <x:c r="C52" s="34" t="s"/>
       <x:c r="D52" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E52" s="36" t="s"/>
       <x:c r="F52" s="37" t="s"/>
@@ -2272,13 +2267,13 @@
     </x:row>
     <x:row r="53" spans="1:11" outlineLevel="3">
       <x:c r="B53" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C53" s="41" t="n">
         <x:v>1283</x:v>
       </x:c>
       <x:c r="D53" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E53" s="42">
         <x:v>34698</x:v>
@@ -2298,7 +2293,7 @@
     </x:row>
     <x:row r="54" spans="1:11" outlineLevel="3">
       <x:c r="B54" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C54" s="41" t="n">
         <x:v>1083</x:v>
@@ -2324,7 +2319,7 @@
       <x:c r="B55" s="34" t="s"/>
       <x:c r="C55" s="34" t="s"/>
       <x:c r="D55" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E55" s="36" t="s"/>
       <x:c r="F55" s="37" t="s"/>
@@ -2336,13 +2331,13 @@
     </x:row>
     <x:row r="56" spans="1:11" outlineLevel="3">
       <x:c r="B56" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C56" s="41" t="n">
         <x:v>1061</x:v>
       </x:c>
       <x:c r="D56" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E56" s="42">
         <x:v>32571</x:v>
@@ -2362,7 +2357,7 @@
     </x:row>
     <x:row r="57" spans="1:11" outlineLevel="3">
       <x:c r="B57" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C57" s="41" t="n">
         <x:v>1057</x:v>
@@ -2386,7 +2381,7 @@
     </x:row>
     <x:row r="58" spans="1:11" outlineLevel="3">
       <x:c r="B58" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C58" s="41" t="n">
         <x:v>1212</x:v>
@@ -2410,7 +2405,7 @@
     </x:row>
     <x:row r="59" spans="1:11" outlineLevel="3">
       <x:c r="B59" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C59" s="41" t="n">
         <x:v>1091</x:v>
@@ -2434,7 +2429,7 @@
     </x:row>
     <x:row r="60" spans="1:11" outlineLevel="3">
       <x:c r="B60" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C60" s="41" t="n">
         <x:v>1261</x:v>
@@ -2458,7 +2453,7 @@
     </x:row>
     <x:row r="61" spans="1:11" outlineLevel="3">
       <x:c r="B61" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C61" s="41" t="n">
         <x:v>1012</x:v>
@@ -2482,7 +2477,7 @@
     </x:row>
     <x:row r="62" spans="1:11" outlineLevel="3">
       <x:c r="B62" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C62" s="41" t="n">
         <x:v>1161</x:v>
@@ -2508,7 +2503,7 @@
       <x:c r="B63" s="34" t="s"/>
       <x:c r="C63" s="34" t="s"/>
       <x:c r="D63" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E63" s="36" t="s"/>
       <x:c r="F63" s="37" t="s"/>
@@ -2520,13 +2515,13 @@
     </x:row>
     <x:row r="64" spans="1:11" outlineLevel="3">
       <x:c r="B64" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C64" s="41" t="n">
         <x:v>1168</x:v>
       </x:c>
       <x:c r="D64" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E64" s="42">
         <x:v>34519</x:v>
@@ -2548,7 +2543,7 @@
       <x:c r="B65" s="34" t="s"/>
       <x:c r="C65" s="34" t="s"/>
       <x:c r="D65" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E65" s="36" t="s"/>
       <x:c r="F65" s="37" t="s"/>
@@ -2560,13 +2555,13 @@
     </x:row>
     <x:row r="66" spans="1:11" outlineLevel="3">
       <x:c r="B66" s="40" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C66" s="41" t="n">
         <x:v>1148</x:v>
       </x:c>
       <x:c r="D66" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E66" s="42">
         <x:v>34396</x:v>
@@ -2586,7 +2581,7 @@
     </x:row>
     <x:row r="67" spans="1:11" outlineLevel="1">
       <x:c r="B67" s="34" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C67" s="34" t="s"/>
       <x:c r="D67" s="35" t="s"/>
@@ -2602,7 +2597,7 @@
       <x:c r="B68" s="34" t="s"/>
       <x:c r="C68" s="34" t="s"/>
       <x:c r="D68" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E68" s="36" t="s"/>
       <x:c r="F68" s="37" t="s"/>
@@ -2614,13 +2609,13 @@
     </x:row>
     <x:row r="69" spans="1:11" outlineLevel="3">
       <x:c r="B69" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C69" s="41" t="n">
         <x:v>1018</x:v>
       </x:c>
       <x:c r="D69" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E69" s="42">
         <x:v>32313</x:v>
@@ -2640,7 +2635,7 @@
     </x:row>
     <x:row r="70" spans="1:11" outlineLevel="3">
       <x:c r="B70" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C70" s="41" t="n">
         <x:v>1118</x:v>
@@ -2666,7 +2661,7 @@
       <x:c r="B71" s="34" t="s"/>
       <x:c r="C71" s="34" t="s"/>
       <x:c r="D71" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E71" s="36" t="s"/>
       <x:c r="F71" s="37" t="s"/>
@@ -2678,13 +2673,13 @@
     </x:row>
     <x:row r="72" spans="1:11" outlineLevel="3">
       <x:c r="B72" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C72" s="41" t="n">
         <x:v>1162</x:v>
       </x:c>
       <x:c r="D72" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E72" s="42">
         <x:v>34494</x:v>
@@ -2704,7 +2699,7 @@
     </x:row>
     <x:row r="73" spans="1:11" outlineLevel="3">
       <x:c r="B73" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C73" s="41" t="n">
         <x:v>1031</x:v>
@@ -2728,7 +2723,7 @@
     </x:row>
     <x:row r="74" spans="1:11" outlineLevel="3">
       <x:c r="B74" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C74" s="41" t="n">
         <x:v>1064</x:v>
@@ -2752,7 +2747,7 @@
     </x:row>
     <x:row r="75" spans="1:11" outlineLevel="3">
       <x:c r="B75" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C75" s="41" t="n">
         <x:v>1131</x:v>
@@ -2776,7 +2771,7 @@
     </x:row>
     <x:row r="76" spans="1:11" outlineLevel="3">
       <x:c r="B76" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C76" s="41" t="n">
         <x:v>1058</x:v>
@@ -2800,7 +2795,7 @@
     </x:row>
     <x:row r="77" spans="1:11" outlineLevel="3">
       <x:c r="B77" s="40" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C77" s="41" t="n">
         <x:v>1062</x:v>
@@ -2824,7 +2819,7 @@
     </x:row>
     <x:row r="78" spans="1:11" outlineLevel="1">
       <x:c r="B78" s="34" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C78" s="34" t="s"/>
       <x:c r="D78" s="35" t="s"/>
@@ -2840,7 +2835,7 @@
       <x:c r="B79" s="34" t="s"/>
       <x:c r="C79" s="34" t="s"/>
       <x:c r="D79" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E79" s="36" t="s"/>
       <x:c r="F79" s="37" t="s"/>
@@ -2852,13 +2847,13 @@
     </x:row>
     <x:row r="80" spans="1:11" outlineLevel="3">
       <x:c r="B80" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C80" s="41" t="n">
         <x:v>1066</x:v>
       </x:c>
       <x:c r="D80" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E80" s="42">
         <x:v>32594</x:v>
@@ -2878,7 +2873,7 @@
     </x:row>
     <x:row r="81" spans="1:11" outlineLevel="3">
       <x:c r="B81" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C81" s="41" t="n">
         <x:v>1205</x:v>
@@ -2902,7 +2897,7 @@
     </x:row>
     <x:row r="82" spans="1:11" outlineLevel="3">
       <x:c r="B82" s="40" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C82" s="41" t="n">
         <x:v>1166</x:v>
@@ -2926,7 +2921,7 @@
     </x:row>
     <x:row r="83" spans="1:11" outlineLevel="1">
       <x:c r="B83" s="34" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C83" s="34" t="s"/>
       <x:c r="D83" s="35" t="s"/>
@@ -2942,7 +2937,7 @@
       <x:c r="B84" s="34" t="s"/>
       <x:c r="C84" s="34" t="s"/>
       <x:c r="D84" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E84" s="36" t="s"/>
       <x:c r="F84" s="37" t="s"/>
@@ -2954,13 +2949,13 @@
     </x:row>
     <x:row r="85" spans="1:11" outlineLevel="3">
       <x:c r="B85" s="40" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C85" s="41" t="n">
         <x:v>1104</x:v>
       </x:c>
       <x:c r="D85" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E85" s="42">
         <x:v>33803</x:v>
@@ -2982,7 +2977,7 @@
       <x:c r="B86" s="34" t="s"/>
       <x:c r="C86" s="34" t="s"/>
       <x:c r="D86" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E86" s="36" t="s"/>
       <x:c r="F86" s="37" t="s"/>
@@ -2994,13 +2989,13 @@
     </x:row>
     <x:row r="87" spans="1:11" outlineLevel="3">
       <x:c r="B87" s="40" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C87" s="41" t="n">
         <x:v>1292</x:v>
       </x:c>
       <x:c r="D87" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E87" s="42">
         <x:v>34700</x:v>
@@ -3020,7 +3015,7 @@
     </x:row>
     <x:row r="88" spans="1:11" outlineLevel="1">
       <x:c r="B88" s="34" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C88" s="34" t="s"/>
       <x:c r="D88" s="35" t="s"/>
@@ -3036,7 +3031,7 @@
       <x:c r="B89" s="34" t="s"/>
       <x:c r="C89" s="34" t="s"/>
       <x:c r="D89" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E89" s="36" t="s"/>
       <x:c r="F89" s="37" t="s"/>
@@ -3048,13 +3043,13 @@
     </x:row>
     <x:row r="90" spans="1:11" outlineLevel="3">
       <x:c r="B90" s="40" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C90" s="41" t="n">
         <x:v>1134</x:v>
       </x:c>
       <x:c r="D90" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E90" s="42">
         <x:v>34287</x:v>
@@ -3074,7 +3069,7 @@
     </x:row>
     <x:row r="91" spans="1:11" outlineLevel="1">
       <x:c r="B91" s="34" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C91" s="34" t="s"/>
       <x:c r="D91" s="35" t="s"/>
@@ -3090,7 +3085,7 @@
       <x:c r="B92" s="34" t="s"/>
       <x:c r="C92" s="34" t="s"/>
       <x:c r="D92" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E92" s="36" t="s"/>
       <x:c r="F92" s="37" t="s"/>
@@ -3102,13 +3097,13 @@
     </x:row>
     <x:row r="93" spans="1:11" outlineLevel="3">
       <x:c r="B93" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C93" s="41" t="n">
         <x:v>1004</x:v>
       </x:c>
       <x:c r="D93" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E93" s="42">
         <x:v>32251</x:v>
@@ -3130,7 +3125,7 @@
       <x:c r="B94" s="34" t="s"/>
       <x:c r="C94" s="34" t="s"/>
       <x:c r="D94" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E94" s="36" t="s"/>
       <x:c r="F94" s="37" t="s"/>
@@ -3142,13 +3137,13 @@
     </x:row>
     <x:row r="95" spans="1:11" outlineLevel="3">
       <x:c r="B95" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C95" s="41" t="n">
         <x:v>1020</x:v>
       </x:c>
       <x:c r="D95" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E95" s="42">
         <x:v>32319</x:v>
@@ -3168,7 +3163,7 @@
     </x:row>
     <x:row r="96" spans="1:11" outlineLevel="3">
       <x:c r="B96" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C96" s="41" t="n">
         <x:v>1120</x:v>
@@ -3194,7 +3189,7 @@
       <x:c r="B97" s="34" t="s"/>
       <x:c r="C97" s="34" t="s"/>
       <x:c r="D97" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E97" s="36" t="s"/>
       <x:c r="F97" s="37" t="s"/>
@@ -3206,13 +3201,13 @@
     </x:row>
     <x:row r="98" spans="1:11" outlineLevel="3">
       <x:c r="B98" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C98" s="41" t="n">
         <x:v>1295</x:v>
       </x:c>
       <x:c r="D98" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E98" s="42">
         <x:v>34705</x:v>
@@ -3232,7 +3227,7 @@
     </x:row>
     <x:row r="99" spans="1:11" outlineLevel="3">
       <x:c r="B99" s="40" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C99" s="41" t="n">
         <x:v>1095</x:v>
@@ -3256,7 +3251,7 @@
     </x:row>
     <x:row r="100" spans="1:11" outlineLevel="1">
       <x:c r="B100" s="34" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C100" s="34" t="s"/>
       <x:c r="D100" s="35" t="s"/>
@@ -3272,7 +3267,7 @@
       <x:c r="B101" s="34" t="s"/>
       <x:c r="C101" s="34" t="s"/>
       <x:c r="D101" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E101" s="36" t="s"/>
       <x:c r="F101" s="37" t="s"/>
@@ -3284,13 +3279,13 @@
     </x:row>
     <x:row r="102" spans="1:11" outlineLevel="3">
       <x:c r="B102" s="40" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C102" s="41" t="n">
         <x:v>1260</x:v>
       </x:c>
       <x:c r="D102" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E102" s="42">
         <x:v>34678</x:v>
@@ -3312,7 +3307,7 @@
       <x:c r="B103" s="34" t="s"/>
       <x:c r="C103" s="34" t="s"/>
       <x:c r="D103" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E103" s="36" t="s"/>
       <x:c r="F103" s="37" t="s"/>
@@ -3324,13 +3319,13 @@
     </x:row>
     <x:row r="104" spans="1:11" outlineLevel="3">
       <x:c r="B104" s="40" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C104" s="41" t="n">
         <x:v>1078</x:v>
       </x:c>
       <x:c r="D104" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E104" s="42">
         <x:v>32630</x:v>
@@ -3350,7 +3345,7 @@
     </x:row>
     <x:row r="105" spans="1:11" outlineLevel="1">
       <x:c r="B105" s="34" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C105" s="34" t="s"/>
       <x:c r="D105" s="35" t="s"/>
@@ -3366,7 +3361,7 @@
       <x:c r="B106" s="34" t="s"/>
       <x:c r="C106" s="34" t="s"/>
       <x:c r="D106" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E106" s="36" t="s"/>
       <x:c r="F106" s="37" t="s"/>
@@ -3378,13 +3373,13 @@
     </x:row>
     <x:row r="107" spans="1:11" outlineLevel="3">
       <x:c r="B107" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C107" s="41" t="n">
         <x:v>1046</x:v>
       </x:c>
       <x:c r="D107" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E107" s="42">
         <x:v>32460</x:v>
@@ -3404,7 +3399,7 @@
     </x:row>
     <x:row r="108" spans="1:11" outlineLevel="3">
       <x:c r="B108" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C108" s="41" t="n">
         <x:v>1146</x:v>
@@ -3430,7 +3425,7 @@
       <x:c r="B109" s="34" t="s"/>
       <x:c r="C109" s="34" t="s"/>
       <x:c r="D109" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E109" s="36" t="s"/>
       <x:c r="F109" s="37" t="s"/>
@@ -3442,13 +3437,13 @@
     </x:row>
     <x:row r="110" spans="1:11" outlineLevel="3">
       <x:c r="B110" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C110" s="41" t="n">
         <x:v>1098</x:v>
       </x:c>
       <x:c r="D110" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E110" s="42">
         <x:v>32673</x:v>
@@ -3468,7 +3463,7 @@
     </x:row>
     <x:row r="111" spans="1:11" outlineLevel="3">
       <x:c r="B111" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C111" s="41" t="n">
         <x:v>1298</x:v>
@@ -3492,7 +3487,7 @@
     </x:row>
     <x:row r="112" spans="1:11" outlineLevel="3">
       <x:c r="B112" s="40" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C112" s="41" t="n">
         <x:v>1198</x:v>
@@ -3516,7 +3511,7 @@
     </x:row>
     <x:row r="113" spans="1:11" outlineLevel="1">
       <x:c r="B113" s="34" t="s">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C113" s="34" t="s"/>
       <x:c r="D113" s="35" t="s"/>
@@ -3532,7 +3527,7 @@
       <x:c r="B114" s="34" t="s"/>
       <x:c r="C114" s="34" t="s"/>
       <x:c r="D114" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E114" s="36" t="s"/>
       <x:c r="F114" s="37" t="s"/>
@@ -3544,13 +3539,13 @@
     </x:row>
     <x:row r="115" spans="1:11" outlineLevel="3">
       <x:c r="B115" s="40" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C115" s="41" t="n">
         <x:v>1130</x:v>
       </x:c>
       <x:c r="D115" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E115" s="42">
         <x:v>34268</x:v>
@@ -3570,7 +3565,7 @@
     </x:row>
     <x:row r="116" spans="1:11" outlineLevel="1">
       <x:c r="B116" s="34" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C116" s="34" t="s"/>
       <x:c r="D116" s="35" t="s"/>
@@ -3586,7 +3581,7 @@
       <x:c r="B117" s="34" t="s"/>
       <x:c r="C117" s="34" t="s"/>
       <x:c r="D117" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E117" s="36" t="s"/>
       <x:c r="F117" s="37" t="s"/>
@@ -3598,13 +3593,13 @@
     </x:row>
     <x:row r="118" spans="1:11" outlineLevel="3">
       <x:c r="B118" s="40" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C118" s="41" t="n">
         <x:v>1048</x:v>
       </x:c>
       <x:c r="D118" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E118" s="42">
         <x:v>32480</x:v>
@@ -3624,7 +3619,7 @@
     </x:row>
     <x:row r="119" spans="1:11" outlineLevel="3">
       <x:c r="B119" s="40" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C119" s="41" t="n">
         <x:v>1054</x:v>
@@ -3648,7 +3643,7 @@
     </x:row>
     <x:row r="120" spans="1:11" outlineLevel="1">
       <x:c r="B120" s="34" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C120" s="34" t="s"/>
       <x:c r="D120" s="35" t="s"/>
@@ -3664,7 +3659,7 @@
       <x:c r="B121" s="34" t="s"/>
       <x:c r="C121" s="34" t="s"/>
       <x:c r="D121" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E121" s="36" t="s"/>
       <x:c r="F121" s="37" t="s"/>
@@ -3676,13 +3671,13 @@
     </x:row>
     <x:row r="122" spans="1:11" outlineLevel="3">
       <x:c r="B122" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C122" s="41" t="n">
         <x:v>1086</x:v>
       </x:c>
       <x:c r="D122" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E122" s="42">
         <x:v>32647</x:v>
@@ -3704,7 +3699,7 @@
       <x:c r="B123" s="34" t="s"/>
       <x:c r="C123" s="34" t="s"/>
       <x:c r="D123" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E123" s="36" t="s"/>
       <x:c r="F123" s="37" t="s"/>
@@ -3716,13 +3711,13 @@
     </x:row>
     <x:row r="124" spans="1:11" outlineLevel="3">
       <x:c r="B124" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C124" s="41" t="n">
         <x:v>1209</x:v>
       </x:c>
       <x:c r="D124" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E124" s="42">
         <x:v>34650</x:v>
@@ -3742,7 +3737,7 @@
     </x:row>
     <x:row r="125" spans="1:11" outlineLevel="3">
       <x:c r="B125" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C125" s="41" t="n">
         <x:v>1109</x:v>
@@ -3766,7 +3761,7 @@
     </x:row>
     <x:row r="126" spans="1:11" outlineLevel="3">
       <x:c r="B126" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C126" s="41" t="n">
         <x:v>1009</x:v>
@@ -3792,7 +3787,7 @@
       <x:c r="B127" s="34" t="s"/>
       <x:c r="C127" s="34" t="s"/>
       <x:c r="D127" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E127" s="36" t="s"/>
       <x:c r="F127" s="37" t="s"/>
@@ -3804,13 +3799,13 @@
     </x:row>
     <x:row r="128" spans="1:11" outlineLevel="3">
       <x:c r="B128" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C128" s="41" t="n">
         <x:v>1090</x:v>
       </x:c>
       <x:c r="D128" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E128" s="42">
         <x:v>32654</x:v>
@@ -3832,7 +3827,7 @@
       <x:c r="B129" s="34" t="s"/>
       <x:c r="C129" s="34" t="s"/>
       <x:c r="D129" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E129" s="36" t="s"/>
       <x:c r="F129" s="37" t="s"/>
@@ -3844,13 +3839,13 @@
     </x:row>
     <x:row r="130" spans="1:11" outlineLevel="3">
       <x:c r="B130" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C130" s="41" t="n">
         <x:v>1056</x:v>
       </x:c>
       <x:c r="D130" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E130" s="42">
         <x:v>32548</x:v>
@@ -3870,7 +3865,7 @@
     </x:row>
     <x:row r="131" spans="1:11" outlineLevel="3">
       <x:c r="B131" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C131" s="41" t="n">
         <x:v>1197</x:v>
@@ -3894,7 +3889,7 @@
     </x:row>
     <x:row r="132" spans="1:11" outlineLevel="3">
       <x:c r="B132" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C132" s="41" t="n">
         <x:v>1156</x:v>
@@ -3920,7 +3915,7 @@
       <x:c r="B133" s="34" t="s"/>
       <x:c r="C133" s="34" t="s"/>
       <x:c r="D133" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E133" s="36" t="s"/>
       <x:c r="F133" s="37" t="s"/>
@@ -3932,13 +3927,13 @@
     </x:row>
     <x:row r="134" spans="1:11" outlineLevel="3">
       <x:c r="B134" s="40" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C134" s="41" t="n">
         <x:v>1165</x:v>
       </x:c>
       <x:c r="D134" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E134" s="42">
         <x:v>34511</x:v>
@@ -3958,7 +3953,7 @@
     </x:row>
     <x:row r="135" spans="1:11" outlineLevel="1">
       <x:c r="B135" s="34" t="s">
-        <x:v>60</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C135" s="34" t="s"/>
       <x:c r="D135" s="35" t="s"/>
@@ -3974,7 +3969,7 @@
       <x:c r="B136" s="34" t="s"/>
       <x:c r="C136" s="34" t="s"/>
       <x:c r="D136" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E136" s="36" t="s"/>
       <x:c r="F136" s="37" t="s"/>
@@ -3986,13 +3981,13 @@
     </x:row>
     <x:row r="137" spans="1:11" outlineLevel="3">
       <x:c r="B137" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C137" s="41" t="n">
         <x:v>1133</x:v>
       </x:c>
       <x:c r="D137" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E137" s="42">
         <x:v>34275</x:v>
@@ -4014,7 +4009,7 @@
       <x:c r="B138" s="34" t="s"/>
       <x:c r="C138" s="34" t="s"/>
       <x:c r="D138" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E138" s="36" t="s"/>
       <x:c r="F138" s="37" t="s"/>
@@ -4026,13 +4021,13 @@
     </x:row>
     <x:row r="139" spans="1:11" outlineLevel="3">
       <x:c r="B139" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C139" s="41" t="n">
         <x:v>1024</x:v>
       </x:c>
       <x:c r="D139" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E139" s="42">
         <x:v>32327</x:v>
@@ -4054,7 +4049,7 @@
       <x:c r="B140" s="34" t="s"/>
       <x:c r="C140" s="34" t="s"/>
       <x:c r="D140" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E140" s="36" t="s"/>
       <x:c r="F140" s="37" t="s"/>
@@ -4066,13 +4061,13 @@
     </x:row>
     <x:row r="141" spans="1:11" outlineLevel="3">
       <x:c r="B141" s="40" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C141" s="41" t="n">
         <x:v>1089</x:v>
       </x:c>
       <x:c r="D141" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E141" s="42">
         <x:v>32651</x:v>
@@ -4092,7 +4087,7 @@
     </x:row>
     <x:row r="142" spans="1:11" outlineLevel="1">
       <x:c r="B142" s="34" t="s">
-        <x:v>62</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C142" s="34" t="s"/>
       <x:c r="D142" s="35" t="s"/>
@@ -4108,7 +4103,7 @@
       <x:c r="B143" s="34" t="s"/>
       <x:c r="C143" s="34" t="s"/>
       <x:c r="D143" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E143" s="36" t="s"/>
       <x:c r="F143" s="37" t="s"/>
@@ -4120,13 +4115,13 @@
     </x:row>
     <x:row r="144" spans="1:11" outlineLevel="3">
       <x:c r="B144" s="40" t="s">
-        <x:v>63</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C144" s="41" t="n">
         <x:v>1019</x:v>
       </x:c>
       <x:c r="D144" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E144" s="42">
         <x:v>32319</x:v>
@@ -4146,7 +4141,7 @@
     </x:row>
     <x:row r="145" spans="1:11" outlineLevel="1">
       <x:c r="B145" s="34" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C145" s="34" t="s"/>
       <x:c r="D145" s="35" t="s"/>
@@ -4162,7 +4157,7 @@
       <x:c r="B146" s="34" t="s"/>
       <x:c r="C146" s="34" t="s"/>
       <x:c r="D146" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E146" s="36" t="s"/>
       <x:c r="F146" s="37" t="s"/>
@@ -4174,13 +4169,13 @@
     </x:row>
     <x:row r="147" spans="1:11" outlineLevel="3">
       <x:c r="B147" s="40" t="s">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C147" s="41" t="n">
         <x:v>1069</x:v>
       </x:c>
       <x:c r="D147" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E147" s="42">
         <x:v>32604</x:v>
@@ -4200,7 +4195,7 @@
     </x:row>
     <x:row r="148" spans="1:11" outlineLevel="1">
       <x:c r="B148" s="34" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C148" s="34" t="s"/>
       <x:c r="D148" s="35" t="s"/>
@@ -4216,7 +4211,7 @@
       <x:c r="B149" s="34" t="s"/>
       <x:c r="C149" s="34" t="s"/>
       <x:c r="D149" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E149" s="36" t="s"/>
       <x:c r="F149" s="37" t="s"/>
@@ -4228,13 +4223,13 @@
     </x:row>
     <x:row r="150" spans="1:11" outlineLevel="3">
       <x:c r="B150" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C150" s="41" t="n">
         <x:v>1081</x:v>
       </x:c>
       <x:c r="D150" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E150" s="42">
         <x:v>32636</x:v>
@@ -4256,7 +4251,7 @@
       <x:c r="B151" s="34" t="s"/>
       <x:c r="C151" s="34" t="s"/>
       <x:c r="D151" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E151" s="36" t="s"/>
       <x:c r="F151" s="37" t="s"/>
@@ -4268,13 +4263,13 @@
     </x:row>
     <x:row r="152" spans="1:11" outlineLevel="3">
       <x:c r="B152" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C152" s="41" t="n">
         <x:v>1103</x:v>
       </x:c>
       <x:c r="D152" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E152" s="42">
         <x:v>33798</x:v>
@@ -4294,7 +4289,7 @@
     </x:row>
     <x:row r="153" spans="1:11" outlineLevel="3">
       <x:c r="B153" s="40" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C153" s="41" t="n">
         <x:v>1063</x:v>
@@ -4318,7 +4313,7 @@
     </x:row>
     <x:row r="154" spans="1:11" outlineLevel="1">
       <x:c r="B154" s="34" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C154" s="34" t="s"/>
       <x:c r="D154" s="35" t="s"/>
@@ -4334,7 +4329,7 @@
       <x:c r="B155" s="34" t="s"/>
       <x:c r="C155" s="34" t="s"/>
       <x:c r="D155" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E155" s="36" t="s"/>
       <x:c r="F155" s="37" t="s"/>
@@ -4346,13 +4341,13 @@
     </x:row>
     <x:row r="156" spans="1:11" outlineLevel="3">
       <x:c r="B156" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C156" s="41" t="n">
         <x:v>1016</x:v>
       </x:c>
       <x:c r="D156" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E156" s="42">
         <x:v>32297</x:v>
@@ -4372,7 +4367,7 @@
     </x:row>
     <x:row r="157" spans="1:11" outlineLevel="3">
       <x:c r="B157" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C157" s="41" t="n">
         <x:v>1116</x:v>
@@ -4398,7 +4393,7 @@
       <x:c r="B158" s="34" t="s"/>
       <x:c r="C158" s="34" t="s"/>
       <x:c r="D158" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E158" s="36" t="s"/>
       <x:c r="F158" s="37" t="s"/>
@@ -4410,13 +4405,13 @@
     </x:row>
     <x:row r="159" spans="1:11" outlineLevel="3">
       <x:c r="B159" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C159" s="41" t="n">
         <x:v>1084</x:v>
       </x:c>
       <x:c r="D159" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E159" s="42">
         <x:v>32640</x:v>
@@ -4438,7 +4433,7 @@
       <x:c r="B160" s="34" t="s"/>
       <x:c r="C160" s="34" t="s"/>
       <x:c r="D160" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E160" s="36" t="s"/>
       <x:c r="F160" s="37" t="s"/>
@@ -4450,13 +4445,13 @@
     </x:row>
     <x:row r="161" spans="1:11" outlineLevel="3">
       <x:c r="B161" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C161" s="41" t="n">
         <x:v>1034</x:v>
       </x:c>
       <x:c r="D161" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E161" s="42">
         <x:v>32369</x:v>
@@ -4478,7 +4473,7 @@
       <x:c r="B162" s="34" t="s"/>
       <x:c r="C162" s="34" t="s"/>
       <x:c r="D162" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E162" s="36" t="s"/>
       <x:c r="F162" s="37" t="s"/>
@@ -4490,13 +4485,13 @@
     </x:row>
     <x:row r="163" spans="1:11" outlineLevel="3">
       <x:c r="B163" s="40" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C163" s="41" t="n">
         <x:v>1093</x:v>
       </x:c>
       <x:c r="D163" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E163" s="42">
         <x:v>32661</x:v>
@@ -4516,7 +4511,7 @@
     </x:row>
     <x:row r="164" spans="1:11" outlineLevel="1">
       <x:c r="B164" s="34" t="s">
-        <x:v>70</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C164" s="34" t="s"/>
       <x:c r="D164" s="35" t="s"/>
@@ -4532,7 +4527,7 @@
       <x:c r="B165" s="34" t="s"/>
       <x:c r="C165" s="34" t="s"/>
       <x:c r="D165" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E165" s="36" t="s"/>
       <x:c r="F165" s="37" t="s"/>
@@ -4544,13 +4539,13 @@
     </x:row>
     <x:row r="166" spans="1:11" outlineLevel="3">
       <x:c r="B166" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C166" s="41" t="n">
         <x:v>1015</x:v>
       </x:c>
       <x:c r="D166" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E166" s="42">
         <x:v>32289</x:v>
@@ -4570,7 +4565,7 @@
     </x:row>
     <x:row r="167" spans="1:11" outlineLevel="3">
       <x:c r="B167" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C167" s="41" t="n">
         <x:v>1315</x:v>
@@ -4594,7 +4589,7 @@
     </x:row>
     <x:row r="168" spans="1:11" outlineLevel="3">
       <x:c r="B168" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C168" s="41" t="n">
         <x:v>1215</x:v>
@@ -4620,7 +4615,7 @@
       <x:c r="B169" s="34" t="s"/>
       <x:c r="C169" s="34" t="s"/>
       <x:c r="D169" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E169" s="36" t="s"/>
       <x:c r="F169" s="37" t="s"/>
@@ -4632,13 +4627,13 @@
     </x:row>
     <x:row r="170" spans="1:11" outlineLevel="3">
       <x:c r="B170" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C170" s="41" t="n">
         <x:v>1128</x:v>
       </x:c>
       <x:c r="D170" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E170" s="42">
         <x:v>34250</x:v>
@@ -4658,7 +4653,7 @@
     </x:row>
     <x:row r="171" spans="1:11" outlineLevel="3">
       <x:c r="B171" s="40" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C171" s="41" t="n">
         <x:v>1028</x:v>
@@ -4682,7 +4677,7 @@
     </x:row>
     <x:row r="172" spans="1:11" outlineLevel="1">
       <x:c r="B172" s="34" t="s">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C172" s="34" t="s"/>
       <x:c r="D172" s="35" t="s"/>
@@ -4698,7 +4693,7 @@
       <x:c r="B173" s="34" t="s"/>
       <x:c r="C173" s="34" t="s"/>
       <x:c r="D173" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E173" s="36" t="s"/>
       <x:c r="F173" s="37" t="s"/>
@@ -4710,13 +4705,13 @@
     </x:row>
     <x:row r="174" spans="1:11" outlineLevel="3">
       <x:c r="B174" s="40" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C174" s="41" t="n">
         <x:v>1141</x:v>
       </x:c>
       <x:c r="D174" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E174" s="42">
         <x:v>34320</x:v>
@@ -4736,7 +4731,7 @@
     </x:row>
     <x:row r="175" spans="1:11" outlineLevel="3">
       <x:c r="B175" s="40" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C175" s="41" t="n">
         <x:v>1041</x:v>
@@ -4760,7 +4755,7 @@
     </x:row>
     <x:row r="176" spans="1:11" outlineLevel="1">
       <x:c r="B176" s="34" t="s">
-        <x:v>74</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C176" s="34" t="s"/>
       <x:c r="D176" s="35" t="s"/>
@@ -4776,7 +4771,7 @@
       <x:c r="B177" s="34" t="s"/>
       <x:c r="C177" s="34" t="s"/>
       <x:c r="D177" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E177" s="36" t="s"/>
       <x:c r="F177" s="37" t="s"/>
@@ -4788,13 +4783,13 @@
     </x:row>
     <x:row r="178" spans="1:11" outlineLevel="3">
       <x:c r="B178" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C178" s="41" t="n">
         <x:v>1023</x:v>
       </x:c>
       <x:c r="D178" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E178" s="42">
         <x:v>32326</x:v>
@@ -4814,7 +4809,7 @@
     </x:row>
     <x:row r="179" spans="1:11" outlineLevel="3">
       <x:c r="B179" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C179" s="41" t="n">
         <x:v>1123</x:v>
@@ -4840,7 +4835,7 @@
       <x:c r="B180" s="34" t="s"/>
       <x:c r="C180" s="34" t="s"/>
       <x:c r="D180" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E180" s="36" t="s"/>
       <x:c r="F180" s="37" t="s"/>
@@ -4852,13 +4847,13 @@
     </x:row>
     <x:row r="181" spans="1:11" outlineLevel="3">
       <x:c r="B181" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C181" s="41" t="n">
         <x:v>1269</x:v>
       </x:c>
       <x:c r="D181" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E181" s="42">
         <x:v>34684</x:v>
@@ -4878,7 +4873,7 @@
     </x:row>
     <x:row r="182" spans="1:11" outlineLevel="3">
       <x:c r="B182" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C182" s="41" t="n">
         <x:v>1169</x:v>
@@ -4904,7 +4899,7 @@
       <x:c r="B183" s="34" t="s"/>
       <x:c r="C183" s="34" t="s"/>
       <x:c r="D183" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E183" s="36" t="s"/>
       <x:c r="F183" s="37" t="s"/>
@@ -4916,13 +4911,13 @@
     </x:row>
     <x:row r="184" spans="1:11" outlineLevel="3">
       <x:c r="B184" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C184" s="41" t="n">
         <x:v>1076</x:v>
       </x:c>
       <x:c r="D184" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E184" s="42">
         <x:v>32624</x:v>
@@ -4942,7 +4937,7 @@
     </x:row>
     <x:row r="185" spans="1:11" outlineLevel="3">
       <x:c r="B185" s="40" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C185" s="41" t="n">
         <x:v>1176</x:v>
@@ -4966,7 +4961,7 @@
     </x:row>
     <x:row r="186" spans="1:11" outlineLevel="1">
       <x:c r="B186" s="34" t="s">
-        <x:v>76</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C186" s="34" t="s"/>
       <x:c r="D186" s="35" t="s"/>
@@ -4982,7 +4977,7 @@
       <x:c r="B187" s="34" t="s"/>
       <x:c r="C187" s="34" t="s"/>
       <x:c r="D187" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E187" s="36" t="s"/>
       <x:c r="F187" s="37" t="s"/>
@@ -4994,13 +4989,13 @@
     </x:row>
     <x:row r="188" spans="1:11" outlineLevel="3">
       <x:c r="B188" s="40" t="s">
-        <x:v>77</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C188" s="41" t="n">
         <x:v>1096</x:v>
       </x:c>
       <x:c r="D188" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E188" s="42">
         <x:v>32668</x:v>
@@ -5020,7 +5015,7 @@
     </x:row>
     <x:row r="189" spans="1:11" outlineLevel="3">
       <x:c r="B189" s="40" t="s">
-        <x:v>77</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C189" s="41" t="n">
         <x:v>1196</x:v>
@@ -5044,7 +5039,7 @@
     </x:row>
     <x:row r="190" spans="1:11" outlineLevel="1">
       <x:c r="B190" s="34" t="s">
-        <x:v>78</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C190" s="34" t="s"/>
       <x:c r="D190" s="35" t="s"/>
@@ -5060,7 +5055,7 @@
       <x:c r="B191" s="34" t="s"/>
       <x:c r="C191" s="34" t="s"/>
       <x:c r="D191" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E191" s="36" t="s"/>
       <x:c r="F191" s="37" t="s"/>
@@ -5072,13 +5067,13 @@
     </x:row>
     <x:row r="192" spans="1:11" outlineLevel="3">
       <x:c r="B192" s="40" t="s">
-        <x:v>79</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C192" s="41" t="n">
         <x:v>1158</x:v>
       </x:c>
       <x:c r="D192" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E192" s="42">
         <x:v>34476</x:v>
@@ -5098,7 +5093,7 @@
     </x:row>
     <x:row r="193" spans="1:11" outlineLevel="1">
       <x:c r="B193" s="34" t="s">
-        <x:v>80</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C193" s="34" t="s"/>
       <x:c r="D193" s="35" t="s"/>
@@ -5114,7 +5109,7 @@
       <x:c r="B194" s="34" t="s"/>
       <x:c r="C194" s="34" t="s"/>
       <x:c r="D194" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E194" s="36" t="s"/>
       <x:c r="F194" s="37" t="s"/>
@@ -5126,13 +5121,13 @@
     </x:row>
     <x:row r="195" spans="1:11" outlineLevel="3">
       <x:c r="B195" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C195" s="41" t="n">
         <x:v>1026</x:v>
       </x:c>
       <x:c r="D195" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E195" s="42">
         <x:v>32332</x:v>
@@ -5152,7 +5147,7 @@
     </x:row>
     <x:row r="196" spans="1:11" outlineLevel="3">
       <x:c r="B196" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C196" s="41" t="n">
         <x:v>1126</x:v>
@@ -5178,7 +5173,7 @@
       <x:c r="B197" s="34" t="s"/>
       <x:c r="C197" s="34" t="s"/>
       <x:c r="D197" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E197" s="36" t="s"/>
       <x:c r="F197" s="37" t="s"/>
@@ -5190,13 +5185,13 @@
     </x:row>
     <x:row r="198" spans="1:11" outlineLevel="3">
       <x:c r="B198" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C198" s="41" t="n">
         <x:v>1013</x:v>
       </x:c>
       <x:c r="D198" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E198" s="42">
         <x:v>32289</x:v>
@@ -5216,7 +5211,7 @@
     </x:row>
     <x:row r="199" spans="1:11" outlineLevel="3">
       <x:c r="B199" s="40" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C199" s="41" t="n">
         <x:v>1113</x:v>
@@ -5240,7 +5235,7 @@
     </x:row>
     <x:row r="200" spans="1:11" outlineLevel="1">
       <x:c r="B200" s="34" t="s">
-        <x:v>82</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C200" s="34" t="s"/>
       <x:c r="D200" s="35" t="s"/>
@@ -5256,7 +5251,7 @@
       <x:c r="B201" s="34" t="s"/>
       <x:c r="C201" s="34" t="s"/>
       <x:c r="D201" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E201" s="36" t="s"/>
       <x:c r="F201" s="37" t="s"/>
@@ -5268,13 +5263,13 @@
     </x:row>
     <x:row r="202" spans="1:11" outlineLevel="3">
       <x:c r="B202" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C202" s="41" t="n">
         <x:v>1860</x:v>
       </x:c>
       <x:c r="D202" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E202" s="42" t="s"/>
       <x:c r="F202" s="42">
@@ -5294,7 +5289,7 @@
       <x:c r="B203" s="34" t="s"/>
       <x:c r="C203" s="34" t="s"/>
       <x:c r="D203" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E203" s="36" t="s"/>
       <x:c r="F203" s="37" t="s"/>
@@ -5306,13 +5301,13 @@
     </x:row>
     <x:row r="204" spans="1:11" outlineLevel="3">
       <x:c r="B204" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C204" s="41" t="n">
         <x:v>1309</x:v>
       </x:c>
       <x:c r="D204" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E204" s="42">
         <x:v>34721</x:v>
@@ -5334,7 +5329,7 @@
       <x:c r="B205" s="34" t="s"/>
       <x:c r="C205" s="34" t="s"/>
       <x:c r="D205" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E205" s="36" t="s"/>
       <x:c r="F205" s="37" t="s"/>
@@ -5346,13 +5341,13 @@
     </x:row>
     <x:row r="206" spans="1:11" outlineLevel="3">
       <x:c r="B206" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C206" s="41" t="n">
         <x:v>1030</x:v>
       </x:c>
       <x:c r="D206" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E206" s="42">
         <x:v>32350</x:v>
@@ -5372,7 +5367,7 @@
     </x:row>
     <x:row r="207" spans="1:11" outlineLevel="3">
       <x:c r="B207" s="40" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C207" s="41" t="n">
         <x:v>1097</x:v>
@@ -5396,7 +5391,7 @@
     </x:row>
     <x:row r="208" spans="1:11" outlineLevel="1">
       <x:c r="B208" s="34" t="s">
-        <x:v>84</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C208" s="34" t="s"/>
       <x:c r="D208" s="35" t="s"/>
@@ -5412,7 +5407,7 @@
       <x:c r="B209" s="34" t="s"/>
       <x:c r="C209" s="34" t="s"/>
       <x:c r="D209" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E209" s="36" t="s"/>
       <x:c r="F209" s="37" t="s"/>
@@ -5424,13 +5419,13 @@
     </x:row>
     <x:row r="210" spans="1:11" outlineLevel="3">
       <x:c r="B210" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C210" s="41" t="n">
         <x:v>1082</x:v>
       </x:c>
       <x:c r="D210" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E210" s="42">
         <x:v>32638</x:v>
@@ -5452,7 +5447,7 @@
       <x:c r="B211" s="34" t="s"/>
       <x:c r="C211" s="34" t="s"/>
       <x:c r="D211" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E211" s="36" t="s"/>
       <x:c r="F211" s="37" t="s"/>
@@ -5464,13 +5459,13 @@
     </x:row>
     <x:row r="212" spans="1:11" outlineLevel="3">
       <x:c r="B212" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C212" s="41" t="n">
         <x:v>1010</x:v>
       </x:c>
       <x:c r="D212" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E212" s="42">
         <x:v>32275</x:v>
@@ -5492,7 +5487,7 @@
       <x:c r="B213" s="34" t="s"/>
       <x:c r="C213" s="34" t="s"/>
       <x:c r="D213" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E213" s="36" t="s"/>
       <x:c r="F213" s="37" t="s"/>
@@ -5504,13 +5499,13 @@
     </x:row>
     <x:row r="214" spans="1:11" outlineLevel="3">
       <x:c r="B214" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C214" s="41" t="n">
         <x:v>1170</x:v>
       </x:c>
       <x:c r="D214" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E214" s="42">
         <x:v>34523</x:v>
@@ -5530,7 +5525,7 @@
     </x:row>
     <x:row r="215" spans="1:11" outlineLevel="3">
       <x:c r="B215" s="40" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C215" s="41" t="n">
         <x:v>1077</x:v>
@@ -5554,7 +5549,7 @@
     </x:row>
     <x:row r="216" spans="1:11" outlineLevel="1">
       <x:c r="B216" s="34" t="s">
-        <x:v>86</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C216" s="34" t="s"/>
       <x:c r="D216" s="35" t="s"/>
@@ -5570,7 +5565,7 @@
       <x:c r="B217" s="34" t="s"/>
       <x:c r="C217" s="34" t="s"/>
       <x:c r="D217" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E217" s="36" t="s"/>
       <x:c r="F217" s="37" t="s"/>
@@ -5582,13 +5577,13 @@
     </x:row>
     <x:row r="218" spans="1:11" outlineLevel="3">
       <x:c r="B218" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C218" s="41" t="n">
         <x:v>1045</x:v>
       </x:c>
       <x:c r="D218" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E218" s="42">
         <x:v>32433</x:v>
@@ -5608,7 +5603,7 @@
     </x:row>
     <x:row r="219" spans="1:11" outlineLevel="3">
       <x:c r="B219" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C219" s="41" t="n">
         <x:v>1145</x:v>
@@ -5634,7 +5629,7 @@
       <x:c r="B220" s="34" t="s"/>
       <x:c r="C220" s="34" t="s"/>
       <x:c r="D220" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E220" s="36" t="s"/>
       <x:c r="F220" s="37" t="s"/>
@@ -5646,13 +5641,13 @@
     </x:row>
     <x:row r="221" spans="1:11" outlineLevel="3">
       <x:c r="B221" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C221" s="41" t="n">
         <x:v>1149</x:v>
       </x:c>
       <x:c r="D221" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E221" s="42">
         <x:v>34407</x:v>
@@ -5672,7 +5667,7 @@
     </x:row>
     <x:row r="222" spans="1:11" outlineLevel="3">
       <x:c r="B222" s="40" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C222" s="41" t="n">
         <x:v>1049</x:v>
@@ -5696,7 +5691,7 @@
     </x:row>
     <x:row r="223" spans="1:11" outlineLevel="1">
       <x:c r="B223" s="34" t="s">
-        <x:v>88</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C223" s="34" t="s"/>
       <x:c r="D223" s="35" t="s"/>
@@ -5712,7 +5707,7 @@
       <x:c r="B224" s="34" t="s"/>
       <x:c r="C224" s="34" t="s"/>
       <x:c r="D224" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E224" s="36" t="s"/>
       <x:c r="F224" s="37" t="s"/>
@@ -5724,13 +5719,13 @@
     </x:row>
     <x:row r="225" spans="1:11" outlineLevel="3">
       <x:c r="B225" s="40" t="s">
-        <x:v>89</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C225" s="41" t="n">
         <x:v>1092</x:v>
       </x:c>
       <x:c r="D225" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E225" s="42">
         <x:v>32660</x:v>
@@ -5750,7 +5745,7 @@
     </x:row>
     <x:row r="226" spans="1:11" outlineLevel="1">
       <x:c r="B226" s="34" t="s">
-        <x:v>90</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C226" s="34" t="s"/>
       <x:c r="D226" s="35" t="s"/>
@@ -5766,7 +5761,7 @@
       <x:c r="B227" s="34" t="s"/>
       <x:c r="C227" s="34" t="s"/>
       <x:c r="D227" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E227" s="36" t="s"/>
       <x:c r="F227" s="37" t="s"/>
@@ -5778,13 +5773,13 @@
     </x:row>
     <x:row r="228" spans="1:11" outlineLevel="3">
       <x:c r="B228" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C228" s="41" t="n">
         <x:v>1047</x:v>
       </x:c>
       <x:c r="D228" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E228" s="42">
         <x:v>32475</x:v>
@@ -5806,7 +5801,7 @@
       <x:c r="B229" s="34" t="s"/>
       <x:c r="C229" s="34" t="s"/>
       <x:c r="D229" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E229" s="36" t="s"/>
       <x:c r="F229" s="37" t="s"/>
@@ -5818,13 +5813,13 @@
     </x:row>
     <x:row r="230" spans="1:11" outlineLevel="3">
       <x:c r="B230" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C230" s="41" t="n">
         <x:v>1144</x:v>
       </x:c>
       <x:c r="D230" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E230" s="42">
         <x:v>34343</x:v>
@@ -5844,7 +5839,7 @@
     </x:row>
     <x:row r="231" spans="1:11" outlineLevel="3">
       <x:c r="B231" s="40" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C231" s="41" t="n">
         <x:v>1044</x:v>
@@ -5868,7 +5863,7 @@
     </x:row>
     <x:row r="232" spans="1:11" outlineLevel="1">
       <x:c r="B232" s="34" t="s">
-        <x:v>92</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C232" s="34" t="s"/>
       <x:c r="D232" s="35" t="s"/>
@@ -5884,7 +5879,7 @@
       <x:c r="B233" s="34" t="s"/>
       <x:c r="C233" s="34" t="s"/>
       <x:c r="D233" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E233" s="36" t="s"/>
       <x:c r="F233" s="37" t="s"/>
@@ -5896,13 +5891,13 @@
     </x:row>
     <x:row r="234" spans="1:11" outlineLevel="3">
       <x:c r="B234" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C234" s="41" t="n">
         <x:v>1025</x:v>
       </x:c>
       <x:c r="D234" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E234" s="42">
         <x:v>32328</x:v>
@@ -5922,7 +5917,7 @@
     </x:row>
     <x:row r="235" spans="1:11" outlineLevel="3">
       <x:c r="B235" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C235" s="41" t="n">
         <x:v>1125</x:v>
@@ -5948,7 +5943,7 @@
       <x:c r="B236" s="34" t="s"/>
       <x:c r="C236" s="34" t="s"/>
       <x:c r="D236" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E236" s="36" t="s"/>
       <x:c r="F236" s="37" t="s"/>
@@ -5960,13 +5955,13 @@
     </x:row>
     <x:row r="237" spans="1:11" outlineLevel="3">
       <x:c r="B237" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C237" s="41" t="n">
         <x:v>1008</x:v>
       </x:c>
       <x:c r="D237" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E237" s="42">
         <x:v>32267</x:v>
@@ -5986,7 +5981,7 @@
     </x:row>
     <x:row r="238" spans="1:11" outlineLevel="3">
       <x:c r="B238" s="40" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C238" s="41" t="n">
         <x:v>1139</x:v>
@@ -6010,7 +6005,7 @@
     </x:row>
     <x:row r="239" spans="1:11" outlineLevel="1">
       <x:c r="B239" s="34" t="s">
-        <x:v>94</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C239" s="34" t="s"/>
       <x:c r="D239" s="35" t="s"/>
@@ -6026,7 +6021,7 @@
       <x:c r="B240" s="34" t="s"/>
       <x:c r="C240" s="34" t="s"/>
       <x:c r="D240" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E240" s="36" t="s"/>
       <x:c r="F240" s="37" t="s"/>
@@ -6038,13 +6033,13 @@
     </x:row>
     <x:row r="241" spans="1:11" outlineLevel="3">
       <x:c r="B241" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C241" s="41" t="n">
         <x:v>1183</x:v>
       </x:c>
       <x:c r="D241" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E241" s="42">
         <x:v>34556</x:v>
@@ -6066,7 +6061,7 @@
       <x:c r="B242" s="34" t="s"/>
       <x:c r="C242" s="34" t="s"/>
       <x:c r="D242" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E242" s="36" t="s"/>
       <x:c r="F242" s="37" t="s"/>
@@ -6078,13 +6073,13 @@
     </x:row>
     <x:row r="243" spans="1:11" outlineLevel="3">
       <x:c r="B243" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C243" s="41" t="n">
         <x:v>1112</x:v>
       </x:c>
       <x:c r="D243" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E243" s="42">
         <x:v>33971</x:v>
@@ -6106,7 +6101,7 @@
       <x:c r="B244" s="34" t="s"/>
       <x:c r="C244" s="34" t="s"/>
       <x:c r="D244" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E244" s="36" t="s"/>
       <x:c r="F244" s="37" t="s"/>
@@ -6118,13 +6113,13 @@
     </x:row>
     <x:row r="245" spans="1:11" outlineLevel="3">
       <x:c r="B245" s="40" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C245" s="41" t="n">
         <x:v>1068</x:v>
       </x:c>
       <x:c r="D245" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E245" s="42">
         <x:v>32602</x:v>
@@ -6144,7 +6139,7 @@
     </x:row>
     <x:row r="246" spans="1:11" outlineLevel="1">
       <x:c r="B246" s="34" t="s">
-        <x:v>96</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C246" s="34" t="s"/>
       <x:c r="D246" s="35" t="s"/>
@@ -6160,7 +6155,7 @@
       <x:c r="B247" s="34" t="s"/>
       <x:c r="C247" s="34" t="s"/>
       <x:c r="D247" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E247" s="36" t="s"/>
       <x:c r="F247" s="37" t="s"/>
@@ -6172,13 +6167,13 @@
     </x:row>
     <x:row r="248" spans="1:11" outlineLevel="3">
       <x:c r="B248" s="40" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C248" s="41" t="n">
         <x:v>1043</x:v>
       </x:c>
       <x:c r="D248" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E248" s="42">
         <x:v>32417</x:v>
@@ -6198,7 +6193,7 @@
     </x:row>
     <x:row r="249" spans="1:11" outlineLevel="3">
       <x:c r="B249" s="40" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C249" s="41" t="n">
         <x:v>1143</x:v>
@@ -6222,7 +6217,7 @@
     </x:row>
     <x:row r="250" spans="1:11" outlineLevel="1">
       <x:c r="B250" s="34" t="s">
-        <x:v>98</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C250" s="34" t="s"/>
       <x:c r="D250" s="35" t="s"/>
@@ -6238,7 +6233,7 @@
       <x:c r="B251" s="34" t="s"/>
       <x:c r="C251" s="34" t="s"/>
       <x:c r="D251" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E251" s="36" t="s"/>
       <x:c r="F251" s="37" t="s"/>
@@ -6250,13 +6245,13 @@
     </x:row>
     <x:row r="252" spans="1:11" outlineLevel="3">
       <x:c r="B252" s="40" t="s">
-        <x:v>99</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C252" s="41" t="n">
         <x:v>1201</x:v>
       </x:c>
       <x:c r="D252" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E252" s="42">
         <x:v>34611</x:v>
@@ -6276,7 +6271,7 @@
     </x:row>
     <x:row r="253" spans="1:11" outlineLevel="1">
       <x:c r="B253" s="34" t="s">
-        <x:v>100</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C253" s="34" t="s"/>
       <x:c r="D253" s="35" t="s"/>
@@ -6292,7 +6287,7 @@
       <x:c r="B254" s="34" t="s"/>
       <x:c r="C254" s="34" t="s"/>
       <x:c r="D254" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E254" s="36" t="s"/>
       <x:c r="F254" s="37" t="s"/>
@@ -6304,13 +6299,13 @@
     </x:row>
     <x:row r="255" spans="1:11" outlineLevel="3">
       <x:c r="B255" s="40" t="s">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C255" s="41" t="n">
         <x:v>1199</x:v>
       </x:c>
       <x:c r="D255" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E255" s="42">
         <x:v>34593</x:v>
@@ -6332,7 +6327,7 @@
       <x:c r="B256" s="34" t="s"/>
       <x:c r="C256" s="34" t="s"/>
       <x:c r="D256" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E256" s="36" t="s"/>
       <x:c r="F256" s="37" t="s"/>
@@ -6344,13 +6339,13 @@
     </x:row>
     <x:row r="257" spans="1:11" outlineLevel="3">
       <x:c r="B257" s="40" t="s">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C257" s="41" t="n">
         <x:v>1094</x:v>
       </x:c>
       <x:c r="D257" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E257" s="42">
         <x:v>32663</x:v>
@@ -6370,7 +6365,7 @@
     </x:row>
     <x:row r="258" spans="1:11" outlineLevel="1">
       <x:c r="B258" s="34" t="s">
-        <x:v>102</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C258" s="34" t="s"/>
       <x:c r="D258" s="35" t="s"/>
@@ -6386,7 +6381,7 @@
       <x:c r="B259" s="34" t="s"/>
       <x:c r="C259" s="34" t="s"/>
       <x:c r="D259" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E259" s="36" t="s"/>
       <x:c r="F259" s="37" t="s"/>
@@ -6398,13 +6393,13 @@
     </x:row>
     <x:row r="260" spans="1:11" outlineLevel="3">
       <x:c r="B260" s="40" t="s">
-        <x:v>103</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C260" s="41" t="n">
         <x:v>1175</x:v>
       </x:c>
       <x:c r="D260" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E260" s="42">
         <x:v>34537</x:v>
@@ -6424,7 +6419,7 @@
     </x:row>
     <x:row r="261" spans="1:11" outlineLevel="1">
       <x:c r="B261" s="34" t="s">
-        <x:v>104</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C261" s="34" t="s"/>
       <x:c r="D261" s="35" t="s"/>
@@ -6440,7 +6435,7 @@
       <x:c r="B262" s="34" t="s"/>
       <x:c r="C262" s="34" t="s"/>
       <x:c r="D262" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E262" s="36" t="s"/>
       <x:c r="F262" s="37" t="s"/>
@@ -6452,13 +6447,13 @@
     </x:row>
     <x:row r="263" spans="1:11" outlineLevel="3">
       <x:c r="B263" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C263" s="41" t="n">
         <x:v>1132</x:v>
       </x:c>
       <x:c r="D263" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E263" s="42">
         <x:v>34274</x:v>
@@ -6478,7 +6473,7 @@
     </x:row>
     <x:row r="264" spans="1:11" outlineLevel="3">
       <x:c r="B264" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C264" s="41" t="n">
         <x:v>1221</x:v>
@@ -6502,7 +6497,7 @@
     </x:row>
     <x:row r="265" spans="1:11" outlineLevel="3">
       <x:c r="B265" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C265" s="41" t="n">
         <x:v>1136</x:v>
@@ -6526,7 +6521,7 @@
     </x:row>
     <x:row r="266" spans="1:11" outlineLevel="3">
       <x:c r="B266" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C266" s="41" t="n">
         <x:v>1021</x:v>
@@ -6550,7 +6545,7 @@
     </x:row>
     <x:row r="267" spans="1:11" outlineLevel="3">
       <x:c r="B267" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C267" s="41" t="n">
         <x:v>1032</x:v>
@@ -6574,7 +6569,7 @@
     </x:row>
     <x:row r="268" spans="1:11" outlineLevel="3">
       <x:c r="B268" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C268" s="41" t="n">
         <x:v>1122</x:v>
@@ -6598,7 +6593,7 @@
     </x:row>
     <x:row r="269" spans="1:11" outlineLevel="3">
       <x:c r="B269" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C269" s="41" t="n">
         <x:v>1121</x:v>
@@ -6622,7 +6617,7 @@
     </x:row>
     <x:row r="270" spans="1:11" outlineLevel="3">
       <x:c r="B270" s="40" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C270" s="41" t="n">
         <x:v>1022</x:v>
@@ -6646,7 +6641,7 @@
     </x:row>
     <x:row r="271" spans="1:11" outlineLevel="1">
       <x:c r="B271" s="34" t="s">
-        <x:v>106</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C271" s="34" t="s"/>
       <x:c r="D271" s="35" t="s"/>
@@ -6662,7 +6657,7 @@
       <x:c r="B272" s="34" t="s"/>
       <x:c r="C272" s="34" t="s"/>
       <x:c r="D272" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E272" s="36" t="s"/>
       <x:c r="F272" s="37" t="s"/>
@@ -6674,13 +6669,13 @@
     </x:row>
     <x:row r="273" spans="1:11" outlineLevel="3">
       <x:c r="B273" s="40" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C273" s="41" t="n">
         <x:v>1101</x:v>
       </x:c>
       <x:c r="D273" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E273" s="42">
         <x:v>32693</x:v>
@@ -6700,7 +6695,7 @@
     </x:row>
     <x:row r="274" spans="1:11" outlineLevel="3">
       <x:c r="B274" s="40" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C274" s="41" t="n">
         <x:v>1051</x:v>
@@ -6724,7 +6719,7 @@
     </x:row>
     <x:row r="275" spans="1:11" outlineLevel="1">
       <x:c r="B275" s="34" t="s">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C275" s="34" t="s"/>
       <x:c r="D275" s="35" t="s"/>
@@ -6740,7 +6735,7 @@
       <x:c r="B276" s="34" t="s"/>
       <x:c r="C276" s="34" t="s"/>
       <x:c r="D276" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E276" s="36" t="s"/>
       <x:c r="F276" s="37" t="s"/>
@@ -6752,13 +6747,13 @@
     </x:row>
     <x:row r="277" spans="1:11" outlineLevel="3">
       <x:c r="B277" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C277" s="41" t="n">
         <x:v>1052</x:v>
       </x:c>
       <x:c r="D277" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E277" s="42">
         <x:v>32515</x:v>
@@ -6778,7 +6773,7 @@
     </x:row>
     <x:row r="278" spans="1:11" outlineLevel="3">
       <x:c r="B278" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C278" s="41" t="n">
         <x:v>1155</x:v>
@@ -6802,7 +6797,7 @@
     </x:row>
     <x:row r="279" spans="1:11" outlineLevel="3">
       <x:c r="B279" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C279" s="41" t="n">
         <x:v>1152</x:v>
@@ -6826,7 +6821,7 @@
     </x:row>
     <x:row r="280" spans="1:11" outlineLevel="3">
       <x:c r="B280" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C280" s="41" t="n">
         <x:v>1163</x:v>
@@ -6850,7 +6845,7 @@
     </x:row>
     <x:row r="281" spans="1:11" outlineLevel="3">
       <x:c r="B281" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C281" s="41" t="n">
         <x:v>1087</x:v>
@@ -6874,7 +6869,7 @@
     </x:row>
     <x:row r="282" spans="1:11" outlineLevel="3">
       <x:c r="B282" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C282" s="41" t="n">
         <x:v>1055</x:v>
@@ -6898,7 +6893,7 @@
     </x:row>
     <x:row r="283" spans="1:11" outlineLevel="3">
       <x:c r="B283" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C283" s="41" t="n">
         <x:v>1003</x:v>
@@ -6922,7 +6917,7 @@
     </x:row>
     <x:row r="284" spans="1:11" outlineLevel="3">
       <x:c r="B284" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C284" s="41" t="n">
         <x:v>1255</x:v>
@@ -6948,7 +6943,7 @@
       <x:c r="B285" s="34" t="s"/>
       <x:c r="C285" s="34" t="s"/>
       <x:c r="D285" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E285" s="36" t="s"/>
       <x:c r="F285" s="37" t="s"/>
@@ -6960,13 +6955,13 @@
     </x:row>
     <x:row r="286" spans="1:11" outlineLevel="3">
       <x:c r="B286" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C286" s="41" t="n">
         <x:v>1275</x:v>
       </x:c>
       <x:c r="D286" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E286" s="42">
         <x:v>34690</x:v>
@@ -6986,7 +6981,7 @@
     </x:row>
     <x:row r="287" spans="1:11" outlineLevel="3">
       <x:c r="B287" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C287" s="41" t="n">
         <x:v>1075</x:v>
@@ -7012,7 +7007,7 @@
       <x:c r="B288" s="34" t="s"/>
       <x:c r="C288" s="34" t="s"/>
       <x:c r="D288" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E288" s="36" t="s"/>
       <x:c r="F288" s="37" t="s"/>
@@ -7024,13 +7019,13 @@
     </x:row>
     <x:row r="289" spans="1:11" outlineLevel="3">
       <x:c r="B289" s="40" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C289" s="41" t="n">
         <x:v>1067</x:v>
       </x:c>
       <x:c r="D289" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E289" s="42">
         <x:v>32600</x:v>
@@ -7050,7 +7045,7 @@
     </x:row>
     <x:row r="290" spans="1:11" outlineLevel="1">
       <x:c r="B290" s="34" t="s">
-        <x:v>110</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C290" s="34" t="s"/>
       <x:c r="D290" s="35" t="s"/>
@@ -7066,7 +7061,7 @@
       <x:c r="B291" s="34" t="s"/>
       <x:c r="C291" s="34" t="s"/>
       <x:c r="D291" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E291" s="36" t="s"/>
       <x:c r="F291" s="37" t="s"/>
@@ -7078,13 +7073,13 @@
     </x:row>
     <x:row r="292" spans="1:11" outlineLevel="3">
       <x:c r="B292" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C292" s="41" t="n">
         <x:v>1171</x:v>
       </x:c>
       <x:c r="D292" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E292" s="42">
         <x:v>34525</x:v>
@@ -7104,7 +7099,7 @@
     </x:row>
     <x:row r="293" spans="1:11" outlineLevel="3">
       <x:c r="B293" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C293" s="41" t="n">
         <x:v>1271</x:v>
@@ -7128,7 +7123,7 @@
     </x:row>
     <x:row r="294" spans="1:11" outlineLevel="3">
       <x:c r="B294" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C294" s="41" t="n">
         <x:v>1071</x:v>
@@ -7154,7 +7149,7 @@
       <x:c r="B295" s="34" t="s"/>
       <x:c r="C295" s="34" t="s"/>
       <x:c r="D295" s="35" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E295" s="36" t="s"/>
       <x:c r="F295" s="37" t="s"/>
@@ -7166,13 +7161,13 @@
     </x:row>
     <x:row r="296" spans="1:11" outlineLevel="3">
       <x:c r="B296" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C296" s="41" t="n">
         <x:v>1011</x:v>
       </x:c>
       <x:c r="D296" s="40" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E296" s="42">
         <x:v>32282</x:v>
@@ -7192,7 +7187,7 @@
     </x:row>
     <x:row r="297" spans="1:11" outlineLevel="3">
       <x:c r="B297" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C297" s="41" t="n">
         <x:v>1111</x:v>
@@ -7218,7 +7213,7 @@
       <x:c r="B298" s="34" t="s"/>
       <x:c r="C298" s="34" t="s"/>
       <x:c r="D298" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E298" s="36" t="s"/>
       <x:c r="F298" s="37" t="s"/>
@@ -7230,13 +7225,13 @@
     </x:row>
     <x:row r="299" spans="1:11" outlineLevel="3">
       <x:c r="B299" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C299" s="41" t="n">
         <x:v>1035</x:v>
       </x:c>
       <x:c r="D299" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E299" s="42">
         <x:v>32372</x:v>
@@ -7258,7 +7253,7 @@
       <x:c r="B300" s="34" t="s"/>
       <x:c r="C300" s="34" t="s"/>
       <x:c r="D300" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E300" s="36" t="s"/>
       <x:c r="F300" s="37" t="s"/>
@@ -7270,13 +7265,13 @@
     </x:row>
     <x:row r="301" spans="1:11" outlineLevel="3">
       <x:c r="B301" s="40" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C301" s="41" t="n">
         <x:v>1154</x:v>
       </x:c>
       <x:c r="D301" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E301" s="42">
         <x:v>34455</x:v>
@@ -7296,7 +7291,7 @@
     </x:row>
     <x:row r="302" spans="1:11" outlineLevel="1">
       <x:c r="B302" s="34" t="s">
-        <x:v>112</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C302" s="34" t="s"/>
       <x:c r="D302" s="35" t="s"/>
@@ -7312,7 +7307,7 @@
       <x:c r="B303" s="34" t="s"/>
       <x:c r="C303" s="34" t="s"/>
       <x:c r="D303" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E303" s="36" t="s"/>
       <x:c r="F303" s="37" t="s"/>
@@ -7324,13 +7319,13 @@
     </x:row>
     <x:row r="304" spans="1:11" outlineLevel="3">
       <x:c r="B304" s="40" t="s">
-        <x:v>113</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C304" s="41" t="n">
         <x:v>1053</x:v>
       </x:c>
       <x:c r="D304" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E304" s="42">
         <x:v>32524</x:v>
@@ -7350,7 +7345,7 @@
     </x:row>
     <x:row r="305" spans="1:11" outlineLevel="1">
       <x:c r="B305" s="34" t="s">
-        <x:v>114</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C305" s="34" t="s"/>
       <x:c r="D305" s="35" t="s"/>
@@ -7366,7 +7361,7 @@
       <x:c r="B306" s="34" t="s"/>
       <x:c r="C306" s="34" t="s"/>
       <x:c r="D306" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E306" s="36" t="s"/>
       <x:c r="F306" s="37" t="s"/>
@@ -7378,13 +7373,13 @@
     </x:row>
     <x:row r="307" spans="1:11" outlineLevel="3">
       <x:c r="B307" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C307" s="41" t="n">
         <x:v>1059</x:v>
       </x:c>
       <x:c r="D307" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E307" s="42">
         <x:v>32564</x:v>
@@ -7404,7 +7399,7 @@
     </x:row>
     <x:row r="308" spans="1:11" outlineLevel="3">
       <x:c r="B308" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C308" s="41" t="n">
         <x:v>1072</x:v>
@@ -7430,7 +7425,7 @@
       <x:c r="B309" s="34" t="s"/>
       <x:c r="C309" s="34" t="s"/>
       <x:c r="D309" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E309" s="36" t="s"/>
       <x:c r="F309" s="37" t="s"/>
@@ -7442,13 +7437,13 @@
     </x:row>
     <x:row r="310" spans="1:11" outlineLevel="3">
       <x:c r="B310" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C310" s="41" t="n">
         <x:v>1280</x:v>
       </x:c>
       <x:c r="D310" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E310" s="42">
         <x:v>34694</x:v>
@@ -7468,7 +7463,7 @@
     </x:row>
     <x:row r="311" spans="1:11" outlineLevel="3">
       <x:c r="B311" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C311" s="41" t="n">
         <x:v>1080</x:v>
@@ -7492,7 +7487,7 @@
     </x:row>
     <x:row r="312" spans="1:11" outlineLevel="3">
       <x:c r="B312" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C312" s="41" t="n">
         <x:v>1180</x:v>
@@ -7518,7 +7513,7 @@
       <x:c r="B313" s="34" t="s"/>
       <x:c r="C313" s="34" t="s"/>
       <x:c r="D313" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E313" s="36" t="s"/>
       <x:c r="F313" s="37" t="s"/>
@@ -7530,13 +7525,13 @@
     </x:row>
     <x:row r="314" spans="1:11" outlineLevel="3">
       <x:c r="B314" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C314" s="41" t="n">
         <x:v>1105</x:v>
       </x:c>
       <x:c r="D314" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E314" s="42">
         <x:v>33806</x:v>
@@ -7556,7 +7551,7 @@
     </x:row>
     <x:row r="315" spans="1:11" outlineLevel="3">
       <x:c r="B315" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C315" s="41" t="n">
         <x:v>1005</x:v>
@@ -7580,7 +7575,7 @@
     </x:row>
     <x:row r="316" spans="1:11" outlineLevel="3">
       <x:c r="B316" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C316" s="41" t="n">
         <x:v>1305</x:v>
@@ -7604,7 +7599,7 @@
     </x:row>
     <x:row r="317" spans="1:11" outlineLevel="3">
       <x:c r="B317" s="40" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C317" s="41" t="n">
         <x:v>1266</x:v>
@@ -7628,7 +7623,7 @@
     </x:row>
     <x:row r="318" spans="1:11" outlineLevel="1">
       <x:c r="B318" s="34" t="s">
-        <x:v>116</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C318" s="34" t="s"/>
       <x:c r="D318" s="35" t="s"/>
@@ -7644,7 +7639,7 @@
       <x:c r="B319" s="34" t="s"/>
       <x:c r="C319" s="34" t="s"/>
       <x:c r="D319" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E319" s="36" t="s"/>
       <x:c r="F319" s="37" t="s"/>
@@ -7656,13 +7651,13 @@
     </x:row>
     <x:row r="320" spans="1:11" outlineLevel="3">
       <x:c r="B320" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C320" s="41" t="n">
         <x:v>1119</x:v>
       </x:c>
       <x:c r="D320" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E320" s="42">
         <x:v>34104</x:v>
@@ -7682,7 +7677,7 @@
     </x:row>
     <x:row r="321" spans="1:11" outlineLevel="3">
       <x:c r="B321" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C321" s="41" t="n">
         <x:v>1036</x:v>
@@ -7708,7 +7703,7 @@
       <x:c r="B322" s="34" t="s"/>
       <x:c r="C322" s="34" t="s"/>
       <x:c r="D322" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E322" s="36" t="s"/>
       <x:c r="F322" s="37" t="s"/>
@@ -7720,13 +7715,13 @@
     </x:row>
     <x:row r="323" spans="1:11" outlineLevel="3">
       <x:c r="B323" s="40" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C323" s="41" t="n">
         <x:v>1195</x:v>
       </x:c>
       <x:c r="D323" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E323" s="42">
         <x:v>34583</x:v>
@@ -7746,7 +7741,7 @@
     </x:row>
     <x:row r="324" spans="1:11" outlineLevel="1">
       <x:c r="B324" s="34" t="s">
-        <x:v>118</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C324" s="34" t="s"/>
       <x:c r="D324" s="35" t="s"/>
@@ -7762,7 +7757,7 @@
       <x:c r="B325" s="34" t="s"/>
       <x:c r="C325" s="34" t="s"/>
       <x:c r="D325" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E325" s="36" t="s"/>
       <x:c r="F325" s="37" t="s"/>
@@ -7774,13 +7769,13 @@
     </x:row>
     <x:row r="326" spans="1:11" outlineLevel="3">
       <x:c r="B326" s="40" t="s">
-        <x:v>119</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C326" s="41" t="n">
         <x:v>1115</x:v>
       </x:c>
       <x:c r="D326" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E326" s="42">
         <x:v>34041</x:v>
@@ -7800,7 +7795,7 @@
     </x:row>
     <x:row r="327" spans="1:11" outlineLevel="1">
       <x:c r="B327" s="34" t="s">
-        <x:v>120</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C327" s="34" t="s"/>
       <x:c r="D327" s="35" t="s"/>
@@ -7816,7 +7811,7 @@
       <x:c r="B328" s="34" t="s"/>
       <x:c r="C328" s="34" t="s"/>
       <x:c r="D328" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E328" s="36" t="s"/>
       <x:c r="F328" s="37" t="s"/>
@@ -7828,13 +7823,13 @@
     </x:row>
     <x:row r="329" spans="1:11" outlineLevel="3">
       <x:c r="B329" s="40" t="s">
-        <x:v>121</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C329" s="41" t="n">
         <x:v>1070</x:v>
       </x:c>
       <x:c r="D329" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E329" s="42">
         <x:v>32606</x:v>
@@ -7854,7 +7849,7 @@
     </x:row>
     <x:row r="330" spans="1:11" outlineLevel="1">
       <x:c r="B330" s="34" t="s">
-        <x:v>122</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C330" s="34" t="s"/>
       <x:c r="D330" s="35" t="s"/>
@@ -7870,7 +7865,7 @@
       <x:c r="B331" s="34" t="s"/>
       <x:c r="C331" s="34" t="s"/>
       <x:c r="D331" s="35" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E331" s="36" t="s"/>
       <x:c r="F331" s="37" t="s"/>
@@ -7882,13 +7877,13 @@
     </x:row>
     <x:row r="332" spans="1:11" outlineLevel="3">
       <x:c r="B332" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C332" s="41" t="n">
         <x:v>1250</x:v>
       </x:c>
       <x:c r="D332" s="40" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E332" s="42">
         <x:v>34662</x:v>
@@ -7908,7 +7903,7 @@
     </x:row>
     <x:row r="333" spans="1:11" outlineLevel="3">
       <x:c r="B333" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C333" s="41" t="n">
         <x:v>1350</x:v>
@@ -7932,7 +7927,7 @@
     </x:row>
     <x:row r="334" spans="1:11" outlineLevel="3">
       <x:c r="B334" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C334" s="41" t="n">
         <x:v>1050</x:v>
@@ -7956,7 +7951,7 @@
     </x:row>
     <x:row r="335" spans="1:11" outlineLevel="3">
       <x:c r="B335" s="40" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C335" s="41" t="n">
         <x:v>1150</x:v>
@@ -7980,7 +7975,7 @@
     </x:row>
     <x:row r="336" spans="1:11" outlineLevel="1">
       <x:c r="B336" s="34" t="s">
-        <x:v>124</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C336" s="34" t="s"/>
       <x:c r="D336" s="35" t="s"/>
@@ -7996,7 +7991,7 @@
       <x:c r="B337" s="34" t="s"/>
       <x:c r="C337" s="34" t="s"/>
       <x:c r="D337" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E337" s="36" t="s"/>
       <x:c r="F337" s="37" t="s"/>
@@ -8008,13 +8003,13 @@
     </x:row>
     <x:row r="338" spans="1:11" outlineLevel="3">
       <x:c r="B338" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C338" s="41" t="n">
         <x:v>1060</x:v>
       </x:c>
       <x:c r="D338" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E338" s="42">
         <x:v>32568</x:v>
@@ -8034,7 +8029,7 @@
     </x:row>
     <x:row r="339" spans="1:11" outlineLevel="3">
       <x:c r="B339" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C339" s="41" t="n">
         <x:v>1160</x:v>
@@ -8060,7 +8055,7 @@
       <x:c r="B340" s="34" t="s"/>
       <x:c r="C340" s="34" t="s"/>
       <x:c r="D340" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E340" s="36" t="s"/>
       <x:c r="F340" s="37" t="s"/>
@@ -8072,13 +8067,13 @@
     </x:row>
     <x:row r="341" spans="1:11" outlineLevel="3">
       <x:c r="B341" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C341" s="41" t="n">
         <x:v>1202</x:v>
       </x:c>
       <x:c r="D341" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E341" s="42">
         <x:v>34613</x:v>
@@ -8098,7 +8093,7 @@
     </x:row>
     <x:row r="342" spans="1:11" outlineLevel="3">
       <x:c r="B342" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C342" s="41" t="n">
         <x:v>1178</x:v>
@@ -8122,7 +8117,7 @@
     </x:row>
     <x:row r="343" spans="1:11" outlineLevel="3">
       <x:c r="B343" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C343" s="41" t="n">
         <x:v>1302</x:v>
@@ -8146,7 +8141,7 @@
     </x:row>
     <x:row r="344" spans="1:11" outlineLevel="3">
       <x:c r="B344" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C344" s="41" t="n">
         <x:v>1278</x:v>
@@ -8170,7 +8165,7 @@
     </x:row>
     <x:row r="345" spans="1:11" outlineLevel="3">
       <x:c r="B345" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C345" s="41" t="n">
         <x:v>1102</x:v>
@@ -8196,7 +8191,7 @@
       <x:c r="B346" s="34" t="s"/>
       <x:c r="C346" s="34" t="s"/>
       <x:c r="D346" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E346" s="36" t="s"/>
       <x:c r="F346" s="37" t="s"/>
@@ -8208,13 +8203,13 @@
     </x:row>
     <x:row r="347" spans="1:11" outlineLevel="3">
       <x:c r="B347" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C347" s="41" t="n">
         <x:v>1073</x:v>
       </x:c>
       <x:c r="D347" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E347" s="42">
         <x:v>32614</x:v>
@@ -8234,7 +8229,7 @@
     </x:row>
     <x:row r="348" spans="1:11" outlineLevel="3">
       <x:c r="B348" s="40" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C348" s="41" t="n">
         <x:v>1173</x:v>
@@ -8258,7 +8253,7 @@
     </x:row>
     <x:row r="349" spans="1:11" outlineLevel="1">
       <x:c r="B349" s="34" t="s">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C349" s="34" t="s"/>
       <x:c r="D349" s="35" t="s"/>
@@ -8274,7 +8269,7 @@
       <x:c r="B350" s="34" t="s"/>
       <x:c r="C350" s="34" t="s"/>
       <x:c r="D350" s="35" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E350" s="36" t="s"/>
       <x:c r="F350" s="37" t="s"/>
@@ -8286,13 +8281,13 @@
     </x:row>
     <x:row r="351" spans="1:11" outlineLevel="3">
       <x:c r="B351" s="40" t="s">
-        <x:v>127</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C351" s="41" t="n">
         <x:v>1296</x:v>
       </x:c>
       <x:c r="D351" s="40" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E351" s="42">
         <x:v>34707</x:v>
@@ -8312,7 +8307,7 @@
     </x:row>
     <x:row r="352" spans="1:11" outlineLevel="1">
       <x:c r="B352" s="34" t="s">
-        <x:v>128</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C352" s="34" t="s"/>
       <x:c r="D352" s="35" t="s"/>
@@ -8328,7 +8323,7 @@
       <x:c r="B353" s="34" t="s"/>
       <x:c r="C353" s="34" t="s"/>
       <x:c r="D353" s="35" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E353" s="36" t="s"/>
       <x:c r="F353" s="37" t="s"/>
@@ -8340,13 +8335,13 @@
     </x:row>
     <x:row r="354" spans="1:11" outlineLevel="3">
       <x:c r="B354" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C354" s="41" t="n">
         <x:v>1033</x:v>
       </x:c>
       <x:c r="D354" s="40" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E354" s="42">
         <x:v>32357</x:v>
@@ -8368,7 +8363,7 @@
       <x:c r="B355" s="34" t="s"/>
       <x:c r="C355" s="34" t="s"/>
       <x:c r="D355" s="35" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E355" s="36" t="s"/>
       <x:c r="F355" s="37" t="s"/>
@@ -8380,13 +8375,13 @@
     </x:row>
     <x:row r="356" spans="1:11" outlineLevel="3">
       <x:c r="B356" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C356" s="41" t="n">
         <x:v>1124</x:v>
       </x:c>
       <x:c r="D356" s="40" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E356" s="42">
         <x:v>34213</x:v>
@@ -8408,7 +8403,7 @@
       <x:c r="B357" s="34" t="s"/>
       <x:c r="C357" s="34" t="s"/>
       <x:c r="D357" s="35" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E357" s="36" t="s"/>
       <x:c r="F357" s="37" t="s"/>
@@ -8420,13 +8415,13 @@
     </x:row>
     <x:row r="358" spans="1:11" outlineLevel="3">
       <x:c r="B358" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C358" s="41" t="n">
         <x:v>1200</x:v>
       </x:c>
       <x:c r="D358" s="40" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E358" s="42">
         <x:v>34597</x:v>
@@ -8446,7 +8441,7 @@
     </x:row>
     <x:row r="359" spans="1:11" outlineLevel="3">
       <x:c r="B359" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C359" s="41" t="n">
         <x:v>1300</x:v>
@@ -8470,7 +8465,7 @@
     </x:row>
     <x:row r="360" spans="1:11" outlineLevel="3">
       <x:c r="B360" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C360" s="41" t="n">
         <x:v>1100</x:v>
@@ -8496,7 +8491,7 @@
       <x:c r="B361" s="34" t="s"/>
       <x:c r="C361" s="34" t="s"/>
       <x:c r="D361" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E361" s="36" t="s"/>
       <x:c r="F361" s="37" t="s"/>
@@ -8508,13 +8503,13 @@
     </x:row>
     <x:row r="362" spans="1:11" outlineLevel="3">
       <x:c r="B362" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C362" s="41" t="n">
         <x:v>1127</x:v>
       </x:c>
       <x:c r="D362" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E362" s="42">
         <x:v>34244</x:v>
@@ -8534,7 +8529,7 @@
     </x:row>
     <x:row r="363" spans="1:11" outlineLevel="3">
       <x:c r="B363" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C363" s="41" t="n">
         <x:v>1207</x:v>
@@ -8558,7 +8553,7 @@
     </x:row>
     <x:row r="364" spans="1:11" outlineLevel="3">
       <x:c r="B364" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C364" s="41" t="n">
         <x:v>1027</x:v>
@@ -8582,7 +8577,7 @@
     </x:row>
     <x:row r="365" spans="1:11" outlineLevel="3">
       <x:c r="B365" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C365" s="41" t="n">
         <x:v>1107</x:v>
@@ -8606,7 +8601,7 @@
     </x:row>
     <x:row r="366" spans="1:11" outlineLevel="3">
       <x:c r="B366" s="40" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C366" s="41" t="n">
         <x:v>1007</x:v>
@@ -8630,7 +8625,7 @@
     </x:row>
     <x:row r="367" spans="1:11" outlineLevel="1">
       <x:c r="B367" s="34" t="s">
-        <x:v>130</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C367" s="34" t="s"/>
       <x:c r="D367" s="35" t="s"/>
@@ -8646,7 +8641,7 @@
       <x:c r="B368" s="34" t="s"/>
       <x:c r="C368" s="34" t="s"/>
       <x:c r="D368" s="35" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E368" s="36" t="s"/>
       <x:c r="F368" s="37" t="s"/>
@@ -8658,13 +8653,13 @@
     </x:row>
     <x:row r="369" spans="1:11" outlineLevel="3">
       <x:c r="B369" s="40" t="s">
-        <x:v>131</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C369" s="41" t="n">
         <x:v>1140</x:v>
       </x:c>
       <x:c r="D369" s="40" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E369" s="42">
         <x:v>34315</x:v>
@@ -8684,7 +8679,7 @@
     </x:row>
     <x:row r="370" spans="1:11" outlineLevel="3">
       <x:c r="B370" s="40" t="s">
-        <x:v>131</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C370" s="41" t="n">
         <x:v>1040</x:v>

</xml_diff>